<commit_message>
Add more logging for ReduceCoins(). Fix Stat reporting text.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D7B38E-6F08-4956-9B79-75A94CCE826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0C5BB88-DC20-4FAC-8810-910BBC038FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2483,23 +2483,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Name='Read_Rules' Content='Read Rules' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt; or &lt;InlineUIContainer&gt;&lt;Button Name='Begin' Content='Begin Game' FontFamily='Courier New'  FontSize='12'&gt; &lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e000a Cal Arath - Barbarian Prince&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r200' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r201' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Barbarian Prince&lt;/Italic&gt; is a dungeon cawler, self-paced, solo game. You play the game in days. Each day starts with your selecting a daily action
- &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, such as traveling to a new hex on the map. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After all events are resolved for your daily action, you must eat your main evening meal as described in the food rules
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, and if in a town, castle, or temple hex; you must also purchase lodging
- &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The game continues until either you are killed or 70 days (10 weeks) elapse. If you have not won before the 70 days ends, the game is automatically lost! You win if you collect 500gp.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You are Cal Arath, rightful heir to the throne of the Northlands Kingdom. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Few humans match your skill with trusty Bonebitter -- Combat=8
-&lt;LineBreak/&gt;Harsh northlands developed your powerful body -- Endurance=9. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Counter Description is found by selecting &lt;Bold&gt;Help | Counter Description...&lt;/Bold&gt; menu. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                &lt;InlineUIContainer&gt;&lt;Image Name='SetupShowStartingWealth' Source='../images/Tutorial1.gif' Height='150'  Width='150'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e000b Starting Wealth&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Alas, in making your escape, you could only grab a few coins. 
@@ -4441,13 +4424,6 @@
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/OrcLeader.gif'  Height='350' Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e057 Troll&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;A hugh stone-skinned troll confonts your party. The troll has combat skill 8, endurance 8, and wealth 15. Furthermore, the troll skin's has regenerative properties. If automatically cures one wound at the end of every other combat round &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you kill the troll, its stone-skin is a valuble item. Whenever you have an opportunity to buy food at a town, castle, temple, or from merchants; you can sell the skin for 50 gold pieces. It is also known that Count Drogat of Drogat Castle will treasure the gift should you manage to get a personal audience with him.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the roll less or equal to your wit and wiles, you strikes first in combat:
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e058 Band of Dwarves&lt;/Bold&gt;
@@ -5076,16 +5052,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;However, the spectre is a magical being and can be stopped using any possession that protects against magic attacks or injury. Click image to continue.
 &lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Spectre1.gif' Height='275'  Width='550' Name='SpectreMagic'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e083 Wild Boar Charges&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;A hugh wide boar charges toward your party. It has surprised you in combat
- &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- The boar normally has combat skill 5 and endurance 5, but its surprise strike is made with combat skill 8 because of its fearsome charge. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Randomly determine which character in your party is the target of this charge.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The boar continues selecting victims until you escape or kill it. If you kill the boar, see  &lt;InlineUIContainer&gt;&lt;Button Content='e083a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                  &lt;InlineUIContainer&gt;&lt;Image Name='Boar' Source='../images/Boar.gif' Height='300'  Width='195'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e083a Wild Boar Defeated&lt;/Bold&gt;
@@ -6823,24 +6789,6 @@
                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Lizard.gif' Name='Lizard' Height='240' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e165 Elven Town&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You discover a hidden town inhabited by elves. Roll one die, subtracting one if you party includes an elf, magician, wizard, or witch. Add one if your party includes a dwarf. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the roll exeeds your wit and wiles, the elves decide you are untrustworthy. You are immediately arrested
- &lt;InlineUIContainer&gt;&lt;Button Content='e060' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. Otherwise, the elves allow you to visit the town.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you are given permission to visit the town, treat it just like a normal town marked on the map for all purposes, including selection fo daily activities
- &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, food
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, and lodging
- &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. Any followers hired in the town
- &lt;InlineUIContainer&gt;&lt;Button Content='r210' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- will be elves.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you return to the hex later in the game, you must roll again to see if the elves still give you permission to visit or arrest you.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Die Roll = &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e166 Elven Fortress&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You discover a hidden castle inhabited by elves. Roll one die subtacting one if you party includes an elf, magician, wizard, or witch. Add one if your party includes a dwarf.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If the roll equals or exceeds your wit and wiles, the elves decide you are unworthy, and your entire party including yourself are arrested
@@ -7372,22 +7320,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Dismiss' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; a random magic user from party to add one to die roll.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll two die and consult list for results:  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r211d Seeking an Audience with the Count Drogat&lt;/Bold&gt;  &lt;InlineUIContainer&gt;&lt;Button Content='r146a' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Count Drogat. Roll two die and consult the list below for results: 
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e061' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 2 You are Count's next victim&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e062' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 Captain of Guard dislikes your haircut&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Meet the daughter of the Count&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e153' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 Encounter Master of Household&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e158' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 6 Confronted by hostile guards&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e161' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 7 Gain audience if have roc beak otherwise arrested&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 8 Seneschal requires a bribe&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Must learn court manners&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e151' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10 Find favor in Count's eye&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e161' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 11 plus - Audience granted&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r211e Seeking an Audience with Lady Aeravir&lt;/Bold&gt;
@@ -8129,6 +8061,74 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Click image to exit game:
 &lt;LineBreak/&gt;   &lt;InlineUIContainer&gt;&lt;Image Name='EndGameExit' Source='../images/DoorClosing.gif' Height='150' Width='75'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e165 Elven Town&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You discover a hidden town inhabited by elves. Roll one die, subtracting one if you party includes an elf, magician, wizard, or witch. Add one if your party includes a dwarf. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the roll exceeds your wit and wiles, the elves decide you are untrustworthy. You are immediately arrested
+ &lt;InlineUIContainer&gt;&lt;Button Content='e060' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. Otherwise, the elves allow you to visit the town.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you are given permission to visit the town, treat it just like a normal town marked on the map for all purposes, including selection fo daily activities
+ &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, food
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, and lodging
+ &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. Any followers hired in the town
+ &lt;InlineUIContainer&gt;&lt;Button Content='r210' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ will be elves.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you return to the hex later in the game, you must roll again to see if the elves still give you permission to visit or arrest you.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Die Roll = &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e057 Troll&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A huge stone-skinned troll confonts your party. The troll has combat skill 8, endurance 8, and wealth 15. Furthermore, the troll skin's has regenerative properties. If automatically cures one wound at the end of every other combat round &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you kill the troll, its stone-skin is a valuble item. Whenever you have an opportunity to buy food at a town, castle, temple, or from merchants; you can sell the skin for 50 gold pieces. It is also known that Count Drogat of Drogat Castle will treasure the gift should you manage to get a personal audience with him.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the roll less or equal to your wit and wiles, you strikes first in combat:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e000a Cal Arath - Barbarian Prince&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r200' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r201' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Barbarian Prince&lt;/Italic&gt; is a dungeon crawler, self-paced, solo game. You play the game in days. Each day starts with your selecting a daily action
+ &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, such as traveling to a new hex on the map. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After all events are resolved for your daily action, you must eat your main evening meal as described in the food rules
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, and if in a town, castle, or temple hex; you must also purchase lodging
+ &lt;InlineUIContainer&gt;&lt;Button Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The game continues until either you are killed or 70 days (10 weeks) elapse. If you have not won before the 70 days ends, the game is automatically lost! You win if you collect 500gp.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You are Cal Arath, rightful heir to the throne of the Northlands Kingdom. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Few humans match your skill with trusty Bonebiter -- Combat=8
+&lt;LineBreak/&gt;Harsh northlands developed your powerful body -- Endurance=9. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Counter Description is found by selecting &lt;Bold&gt;Help | Counter Description...&lt;/Bold&gt; menu. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                                &lt;InlineUIContainer&gt;&lt;Image Name='SetupShowStartingWealth' Source='../images/Tutorial1.gif' Height='150'  Width='150'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e083 Wild Boar Charges&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A huge wild boar charges toward your party. It has surprised you in combat
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ The boar normally has combat skill 5 and endurance 5, but its surprise strike is made with combat skill 8 because of its fearsome charge. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Randomly determine which character in your party is the target of this charge.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The boar continues selecting victims until you escape or kill it. If you kill the boar, see  &lt;InlineUIContainer&gt;&lt;Button Content='e083a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                  &lt;InlineUIContainer&gt;&lt;Image Name='Boar' Source='../images/Boar.gif' Height='300'  Width='195'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e211d Seeking an Audience with the Count Drogat&lt;/Bold&gt;  &lt;InlineUIContainer&gt;&lt;Button Content='r146a' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Count Drogat. Roll two die and consult the list below for results: 
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e061' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 2 You are Count's next victim&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e062' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 Captain of Guard dislikes your haircut&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Meet the daughter of the Count&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e153' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 Encounter Master of Household&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e158' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 6 Confronted by hostile guards&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e161' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 7 Gain audience if have roc beak otherwise arrested&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 8 Seneschal requires a bribe&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Must learn court manners&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e151' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10 Find favor in Count's eye&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e161' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 11 plus - Audience granted&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -8523,8 +8523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B489" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B490" sqref="B490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8546,7 +8546,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>659</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8554,7 +8554,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8562,7 +8562,7 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8586,7 +8586,7 @@
         <v>655</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8594,7 +8594,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8602,7 +8602,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8610,7 +8610,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8618,7 +8618,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8626,7 +8626,7 @@
         <v>258</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8642,7 +8642,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8650,7 +8650,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8658,7 +8658,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -8666,7 +8666,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8674,7 +8674,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8682,7 +8682,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8690,7 +8690,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8698,7 +8698,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8706,7 +8706,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8714,7 +8714,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8722,7 +8722,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8730,7 +8730,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8738,7 +8738,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -8746,7 +8746,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8754,7 +8754,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8762,7 +8762,7 @@
         <v>261</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8770,7 +8770,7 @@
         <v>546</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8778,7 +8778,7 @@
         <v>547</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8786,7 +8786,7 @@
         <v>549</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8794,7 +8794,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8802,7 +8802,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8810,7 +8810,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8818,7 +8818,7 @@
         <v>551</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8826,7 +8826,7 @@
         <v>552</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8834,7 +8834,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8842,7 +8842,7 @@
         <v>558</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8850,7 +8850,7 @@
         <v>559</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8858,7 +8858,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8866,7 +8866,7 @@
         <v>262</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8874,7 +8874,7 @@
         <v>263</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8882,7 +8882,7 @@
         <v>27</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -8890,7 +8890,7 @@
         <v>28</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -8898,7 +8898,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8906,7 +8906,7 @@
         <v>30</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8914,7 +8914,7 @@
         <v>408</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8922,7 +8922,7 @@
         <v>503</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8930,7 +8930,7 @@
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8938,7 +8938,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8946,7 +8946,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8954,7 +8954,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8962,7 +8962,7 @@
         <v>409</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8970,7 +8970,7 @@
         <v>410</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8978,7 +8978,7 @@
         <v>401</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8986,7 +8986,7 @@
         <v>402</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8994,7 +8994,7 @@
         <v>403</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9002,7 +9002,7 @@
         <v>264</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9010,7 +9010,7 @@
         <v>265</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9018,7 +9018,7 @@
         <v>405</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9026,7 +9026,7 @@
         <v>427</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9034,7 +9034,7 @@
         <v>35</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9042,7 +9042,7 @@
         <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>406</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9058,7 +9058,7 @@
         <v>407</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9066,7 +9066,7 @@
         <v>37</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -9082,7 +9082,7 @@
         <v>43</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9090,7 +9090,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9098,7 +9098,7 @@
         <v>504</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9106,7 +9106,7 @@
         <v>505</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9114,7 +9114,7 @@
         <v>39</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -9122,7 +9122,7 @@
         <v>40</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9130,7 +9130,7 @@
         <v>41</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9138,7 +9138,7 @@
         <v>45</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9146,7 +9146,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9154,7 +9154,7 @@
         <v>46</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9162,7 +9162,7 @@
         <v>47</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9170,7 +9170,7 @@
         <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9178,7 +9178,7 @@
         <v>49</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9186,7 +9186,7 @@
         <v>50</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9194,7 +9194,7 @@
         <v>51</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9202,7 +9202,7 @@
         <v>52</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9210,7 +9210,7 @@
         <v>53</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -9218,7 +9218,7 @@
         <v>54</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9226,7 +9226,7 @@
         <v>55</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9234,7 +9234,7 @@
         <v>56</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9242,7 +9242,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9250,7 +9250,7 @@
         <v>58</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9258,7 +9258,7 @@
         <v>524</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9266,7 +9266,7 @@
         <v>525</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9274,7 +9274,7 @@
         <v>528</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9282,7 +9282,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9290,7 +9290,7 @@
         <v>557</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9298,7 +9298,7 @@
         <v>60</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9306,7 +9306,7 @@
         <v>523</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9314,7 +9314,7 @@
         <v>61</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9322,7 +9322,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9330,7 +9330,7 @@
         <v>342</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9338,7 +9338,7 @@
         <v>63</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -9346,7 +9346,7 @@
         <v>64</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9354,7 +9354,7 @@
         <v>65</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9362,7 +9362,7 @@
         <v>66</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9370,7 +9370,7 @@
         <v>330</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9378,7 +9378,7 @@
         <v>67</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9386,7 +9386,7 @@
         <v>387</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9394,7 +9394,7 @@
         <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9402,7 +9402,7 @@
         <v>343</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9410,7 +9410,7 @@
         <v>388</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9418,7 +9418,7 @@
         <v>69</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9426,7 +9426,7 @@
         <v>391</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9434,7 +9434,7 @@
         <v>392</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9442,7 +9442,7 @@
         <v>70</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -9450,7 +9450,7 @@
         <v>344</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9458,7 +9458,7 @@
         <v>259</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9466,7 +9466,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9474,7 +9474,7 @@
         <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9482,7 +9482,7 @@
         <v>73</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9498,7 +9498,7 @@
         <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9514,7 +9514,7 @@
         <v>325</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9522,7 +9522,7 @@
         <v>622</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9530,7 +9530,7 @@
         <v>76</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9538,7 +9538,7 @@
         <v>77</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9562,7 +9562,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9570,7 +9570,7 @@
         <v>350</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9578,7 +9578,7 @@
         <v>351</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9586,7 +9586,7 @@
         <v>79</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9594,7 +9594,7 @@
         <v>347</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9602,7 +9602,7 @@
         <v>348</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9610,7 +9610,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9618,7 +9618,7 @@
         <v>81</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9626,7 +9626,7 @@
         <v>569</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9634,7 +9634,7 @@
         <v>570</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9642,7 +9642,7 @@
         <v>571</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9650,7 +9650,7 @@
         <v>572</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9658,7 +9658,7 @@
         <v>573</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9666,7 +9666,7 @@
         <v>574</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9674,7 +9674,7 @@
         <v>575</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9682,7 +9682,7 @@
         <v>576</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9690,7 +9690,7 @@
         <v>577</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9698,7 +9698,7 @@
         <v>578</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9706,7 +9706,7 @@
         <v>82</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9714,7 +9714,7 @@
         <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9722,7 +9722,7 @@
         <v>602</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9730,7 +9730,7 @@
         <v>84</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9738,7 +9738,7 @@
         <v>85</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9746,7 +9746,7 @@
         <v>426</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9754,7 +9754,7 @@
         <v>635</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9762,7 +9762,7 @@
         <v>86</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9770,7 +9770,7 @@
         <v>87</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9778,7 +9778,7 @@
         <v>334</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9786,7 +9786,7 @@
         <v>371</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -9794,7 +9794,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9802,7 +9802,7 @@
         <v>335</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9810,7 +9810,7 @@
         <v>336</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9818,7 +9818,7 @@
         <v>337</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9826,7 +9826,7 @@
         <v>339</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9834,7 +9834,7 @@
         <v>338</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9842,7 +9842,7 @@
         <v>340</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9850,7 +9850,7 @@
         <v>341</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9858,7 +9858,7 @@
         <v>510</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9866,7 +9866,7 @@
         <v>89</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9874,7 +9874,7 @@
         <v>376</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9882,7 +9882,7 @@
         <v>377</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9890,7 +9890,7 @@
         <v>380</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9898,7 +9898,7 @@
         <v>90</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9906,7 +9906,7 @@
         <v>536</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9914,7 +9914,7 @@
         <v>537</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9922,7 +9922,7 @@
         <v>91</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9930,7 +9930,7 @@
         <v>381</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9938,7 +9938,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>825</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9946,7 +9946,7 @@
         <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9970,7 +9970,7 @@
         <v>96</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9978,7 +9978,7 @@
         <v>541</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9986,7 +9986,7 @@
         <v>542</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9994,7 +9994,7 @@
         <v>543</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10002,7 +10002,7 @@
         <v>544</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10010,7 +10010,7 @@
         <v>548</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10026,7 +10026,7 @@
         <v>97</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10034,7 +10034,7 @@
         <v>98</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10042,7 +10042,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10050,7 +10050,7 @@
         <v>101</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10058,7 +10058,7 @@
         <v>100</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10066,7 +10066,7 @@
         <v>102</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10074,7 +10074,7 @@
         <v>103</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10082,7 +10082,7 @@
         <v>104</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10090,7 +10090,7 @@
         <v>105</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10098,7 +10098,7 @@
         <v>501</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10106,7 +10106,7 @@
         <v>502</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10114,7 +10114,7 @@
         <v>106</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10122,7 +10122,7 @@
         <v>107</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10130,7 +10130,7 @@
         <v>165</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10138,7 +10138,7 @@
         <v>538</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10146,7 +10146,7 @@
         <v>108</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -10154,7 +10154,7 @@
         <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10162,7 +10162,7 @@
         <v>110</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10170,7 +10170,7 @@
         <v>166</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10178,7 +10178,7 @@
         <v>167</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10186,7 +10186,7 @@
         <v>168</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10194,7 +10194,7 @@
         <v>553</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10210,7 +10210,7 @@
         <v>111</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10218,7 +10218,7 @@
         <v>507</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10226,7 +10226,7 @@
         <v>508</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10242,7 +10242,7 @@
         <v>513</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10250,7 +10250,7 @@
         <v>112</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10258,7 +10258,7 @@
         <v>169</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10266,7 +10266,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10274,7 +10274,7 @@
         <v>171</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10282,7 +10282,7 @@
         <v>113</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10290,7 +10290,7 @@
         <v>114</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10298,7 +10298,7 @@
         <v>266</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10306,7 +10306,7 @@
         <v>560</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10314,7 +10314,7 @@
         <v>115</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10322,7 +10322,7 @@
         <v>519</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10330,7 +10330,7 @@
         <v>116</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10338,7 +10338,7 @@
         <v>517</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10346,7 +10346,7 @@
         <v>117</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10354,7 +10354,7 @@
         <v>520</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10362,7 +10362,7 @@
         <v>521</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10370,7 +10370,7 @@
         <v>522</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10378,7 +10378,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10386,7 +10386,7 @@
         <v>563</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10394,7 +10394,7 @@
         <v>564</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10402,7 +10402,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10410,7 +10410,7 @@
         <v>556</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10418,7 +10418,7 @@
         <v>555</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10426,7 +10426,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10434,7 +10434,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10442,7 +10442,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10450,7 +10450,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10458,7 +10458,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10466,7 +10466,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>886</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10474,7 +10474,7 @@
         <v>518</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10482,7 +10482,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10490,7 +10490,7 @@
         <v>561</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10498,7 +10498,7 @@
         <v>562</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10506,7 +10506,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10514,7 +10514,7 @@
         <v>605</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10522,7 +10522,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10530,7 +10530,7 @@
         <v>579</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10538,7 +10538,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10546,7 +10546,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10554,7 +10554,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10562,7 +10562,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10570,7 +10570,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10578,7 +10578,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10586,7 +10586,7 @@
         <v>566</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10594,7 +10594,7 @@
         <v>567</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10602,7 +10602,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10610,7 +10610,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10618,7 +10618,7 @@
         <v>565</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10626,7 +10626,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10634,7 +10634,7 @@
         <v>580</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10642,7 +10642,7 @@
         <v>581</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10650,7 +10650,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10658,7 +10658,7 @@
         <v>582</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10666,7 +10666,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10682,7 +10682,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10690,7 +10690,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10706,7 +10706,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10714,7 +10714,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10730,7 +10730,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10738,7 +10738,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10746,7 +10746,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10762,7 +10762,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10770,7 +10770,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10778,7 +10778,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10786,7 +10786,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10794,7 +10794,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10802,7 +10802,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10810,7 +10810,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10818,7 +10818,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10826,7 +10826,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10834,7 +10834,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10842,7 +10842,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10850,7 +10850,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10858,7 +10858,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10866,7 +10866,7 @@
         <v>593</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10874,7 +10874,7 @@
         <v>592</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10882,7 +10882,7 @@
         <v>594</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10890,7 +10890,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10898,7 +10898,7 @@
         <v>595</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10906,7 +10906,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10914,7 +10914,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10922,7 +10922,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10930,7 +10930,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10938,7 +10938,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10946,7 +10946,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10954,7 +10954,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10962,7 +10962,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10970,7 +10970,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10986,7 +10986,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10994,7 +10994,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11002,7 +11002,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11026,7 +11026,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11034,7 +11034,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11042,7 +11042,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11050,7 +11050,7 @@
         <v>588</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11058,7 +11058,7 @@
         <v>589</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11066,7 +11066,7 @@
         <v>590</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11074,7 +11074,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11082,7 +11082,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11090,7 +11090,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11098,7 +11098,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11106,7 +11106,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11122,7 +11122,7 @@
         <v>412</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11130,7 +11130,7 @@
         <v>413</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11138,7 +11138,7 @@
         <v>414</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11146,7 +11146,7 @@
         <v>415</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11154,7 +11154,7 @@
         <v>416</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11162,7 +11162,7 @@
         <v>601</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11170,7 +11170,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11186,7 +11186,7 @@
         <v>424</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11194,7 +11194,7 @@
         <v>425</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11202,7 +11202,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11210,7 +11210,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11218,7 +11218,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11226,7 +11226,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11234,7 +11234,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11242,7 +11242,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11250,7 +11250,7 @@
         <v>539</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11258,7 +11258,7 @@
         <v>540</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11266,7 +11266,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11274,7 +11274,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11282,7 +11282,7 @@
         <v>385</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11298,7 +11298,7 @@
         <v>610</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11306,7 +11306,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11314,7 +11314,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11330,7 +11330,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11338,7 +11338,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11346,7 +11346,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11362,7 +11362,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11370,7 +11370,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11378,7 +11378,7 @@
         <v>382</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11386,7 +11386,7 @@
         <v>383</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11394,7 +11394,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11402,7 +11402,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11410,7 +11410,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11418,7 +11418,7 @@
         <v>462</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11426,7 +11426,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11442,7 +11442,7 @@
         <v>333</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11450,7 +11450,7 @@
         <v>612</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11458,7 +11458,7 @@
         <v>613</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11466,7 +11466,7 @@
         <v>615</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11474,7 +11474,7 @@
         <v>616</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11482,7 +11482,7 @@
         <v>617</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11490,7 +11490,7 @@
         <v>618</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11498,7 +11498,7 @@
         <v>619</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11506,7 +11506,7 @@
         <v>620</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11514,7 +11514,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11522,7 +11522,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11530,7 +11530,7 @@
         <v>608</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11538,7 +11538,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11546,7 +11546,7 @@
         <v>328</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11554,7 +11554,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11562,7 +11562,7 @@
         <v>484</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11570,7 +11570,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11578,7 +11578,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11586,7 +11586,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11594,7 +11594,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11602,7 +11602,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11610,7 +11610,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11658,7 +11658,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11666,7 +11666,7 @@
         <v>456</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11674,7 +11674,7 @@
         <v>457</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11682,7 +11682,7 @@
         <v>458</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11690,7 +11690,7 @@
         <v>459</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11698,7 +11698,7 @@
         <v>460</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11706,7 +11706,7 @@
         <v>461</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11714,7 +11714,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11786,7 +11786,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11794,7 +11794,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11802,7 +11802,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11810,7 +11810,7 @@
         <v>473</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11818,7 +11818,7 @@
         <v>474</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11826,7 +11826,7 @@
         <v>475</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11834,7 +11834,7 @@
         <v>476</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11842,7 +11842,7 @@
         <v>477</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11850,7 +11850,7 @@
         <v>478</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11858,7 +11858,7 @@
         <v>609</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11866,7 +11866,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11874,7 +11874,7 @@
         <v>466</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11882,7 +11882,7 @@
         <v>467</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11890,7 +11890,7 @@
         <v>468</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11898,7 +11898,7 @@
         <v>469</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11906,7 +11906,7 @@
         <v>470</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11914,7 +11914,7 @@
         <v>471</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11922,7 +11922,7 @@
         <v>472</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11930,7 +11930,7 @@
         <v>607</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11938,7 +11938,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11946,7 +11946,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11954,7 +11954,7 @@
         <v>417</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11962,7 +11962,7 @@
         <v>418</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11970,7 +11970,7 @@
         <v>419</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11978,7 +11978,7 @@
         <v>420</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11986,7 +11986,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11994,7 +11994,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1053</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12002,7 +12002,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12010,7 +12010,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12018,7 +12018,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12026,7 +12026,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12034,7 +12034,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12042,7 +12042,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12050,7 +12050,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12058,7 +12058,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12066,7 +12066,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12074,7 +12074,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12082,7 +12082,7 @@
         <v>329</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12090,7 +12090,7 @@
         <v>384</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12098,7 +12098,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12106,7 +12106,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -12114,7 +12114,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12122,7 +12122,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12130,7 +12130,7 @@
         <v>606</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12138,7 +12138,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12146,7 +12146,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12154,7 +12154,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12162,7 +12162,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12170,7 +12170,7 @@
         <v>378</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12178,7 +12178,7 @@
         <v>379</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12186,7 +12186,7 @@
         <v>441</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12202,7 +12202,7 @@
         <v>526</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12250,7 +12250,7 @@
         <v>591</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12258,7 +12258,7 @@
         <v>322</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12266,7 +12266,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12274,7 +12274,7 @@
         <v>393</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12282,7 +12282,7 @@
         <v>395</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12290,7 +12290,7 @@
         <v>396</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12298,7 +12298,7 @@
         <v>397</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12306,7 +12306,7 @@
         <v>398</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12314,7 +12314,7 @@
         <v>399</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12322,7 +12322,7 @@
         <v>428</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12330,7 +12330,7 @@
         <v>429</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12338,7 +12338,7 @@
         <v>634</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12346,7 +12346,7 @@
         <v>430</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12354,7 +12354,7 @@
         <v>431</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12362,7 +12362,7 @@
         <v>432</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12370,7 +12370,7 @@
         <v>433</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12378,7 +12378,7 @@
         <v>434</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12386,7 +12386,7 @@
         <v>435</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12394,7 +12394,7 @@
         <v>436</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12402,7 +12402,7 @@
         <v>437</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12410,7 +12410,7 @@
         <v>438</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12418,7 +12418,7 @@
         <v>439</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12426,7 +12426,7 @@
         <v>440</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12434,7 +12434,7 @@
         <v>455</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12442,7 +12442,7 @@
         <v>463</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12450,7 +12450,7 @@
         <v>464</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1104</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12458,7 +12458,7 @@
         <v>465</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1105</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12466,7 +12466,7 @@
         <v>545</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1106</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12474,7 +12474,7 @@
         <v>621</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1107</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12482,7 +12482,7 @@
         <v>485</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1108</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12490,7 +12490,7 @@
         <v>486</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12498,7 +12498,7 @@
         <v>487</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>488</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12514,7 +12514,7 @@
         <v>489</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12522,7 +12522,7 @@
         <v>490</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12530,7 +12530,7 @@
         <v>491</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12538,7 +12538,7 @@
         <v>492</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12546,7 +12546,7 @@
         <v>493</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12554,7 +12554,7 @@
         <v>494</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12562,7 +12562,7 @@
         <v>495</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12570,7 +12570,7 @@
         <v>496</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1119</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12578,7 +12578,7 @@
         <v>497</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12586,7 +12586,7 @@
         <v>498</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12594,7 +12594,7 @@
         <v>499</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12602,7 +12602,7 @@
         <v>586</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12610,7 +12610,7 @@
         <v>587</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1124</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12618,7 +12618,7 @@
         <v>500</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12626,7 +12626,7 @@
         <v>512</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12634,7 +12634,7 @@
         <v>421</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12658,7 +12658,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12666,7 +12666,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12674,7 +12674,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12682,7 +12682,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12690,7 +12690,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12698,7 +12698,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12706,7 +12706,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12714,7 +12714,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12722,7 +12722,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12730,7 +12730,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12738,7 +12738,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12818,7 +12818,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12826,7 +12826,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1140</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12842,7 +12842,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1141</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12850,7 +12850,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1142</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12858,7 +12858,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12866,7 +12866,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1144</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12914,7 +12914,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1145</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12922,7 +12922,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12930,7 +12930,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12938,7 +12938,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1148</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12946,7 +12946,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12954,7 +12954,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12962,7 +12962,7 @@
         <v>353</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12970,7 +12970,7 @@
         <v>365</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1152</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12978,7 +12978,7 @@
         <v>366</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1153</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12986,7 +12986,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1154</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12994,7 +12994,7 @@
         <v>364</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1155</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -13002,7 +13002,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13010,7 +13010,7 @@
         <v>354</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1157</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13026,7 +13026,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13034,7 +13034,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1159</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13042,7 +13042,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13050,7 +13050,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1161</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13058,7 +13058,7 @@
         <v>363</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13066,7 +13066,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13074,7 +13074,7 @@
         <v>361</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13090,7 +13090,7 @@
         <v>514</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13098,7 +13098,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13106,7 +13106,7 @@
         <v>358</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13114,7 +13114,7 @@
         <v>359</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13130,7 +13130,7 @@
         <v>515</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13138,7 +13138,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13146,7 +13146,7 @@
         <v>352</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13154,7 +13154,7 @@
         <v>355</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13162,7 +13162,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13170,7 +13170,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13194,7 +13194,7 @@
         <v>349</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13202,7 +13202,7 @@
         <v>516</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -13210,7 +13210,7 @@
         <v>326</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13234,7 +13234,7 @@
         <v>651</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13250,7 +13250,7 @@
         <v>652</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Game End Stats.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0C5BB88-DC20-4FAC-8810-910BBC038FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8413763C-D017-4626-88C8-7A9AA34C9E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -5043,17 +5043,6 @@
                               &lt;InlineUIContainer&gt;&lt;Image Name='E081EncounterFight' Source='../images/MountedPatrol.gif' Height='250' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e082 Spectre&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;An unearthly spectre from the astal plan appears in the midst of your party casting a hideous miama in all directions.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;One character in the party is the spectre's victim
- &lt;InlineUIContainer&gt;&lt;Button Content='r343' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. It must be a magician, wizard, witch, priest, or monk if they are in your party.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The victim is turned into smoke and taken by the spectre to the astral plane never to be seen again. If you are the victim, the game is lost.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;However, the spectre is a magical being and can be stopped using any possession that protects against magic attacks or injury. Click image to continue.
-&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Image Source='../images/Spectre1.gif' Height='275'  Width='550' Name='SpectreMagic'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e083a Wild Boar Defeated&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Boars are quite delicious!
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll two dice for the number of food units it provides: &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21' &gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8129,6 +8118,17 @@
   &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Must learn court manners&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e151' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10 Find favor in Count's eye&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Content='e161' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 11 plus - Audience granted&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e082 Spectre&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;An unearthly spectre from the astral plan appears in the midst of your party casting a hideous miama in all directions.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;One character in the party is the spectre's victim
+ &lt;InlineUIContainer&gt;&lt;Button Content='r343' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. It must be a magician, wizard, witch, priest, or monk if they are in your party.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The victim is turned into smoke and taken by the spectre to the astral plane never to be seen again. If you are the victim, the game is lost.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;However, the spectre is a magical being and can be stopped using any possession that protects against magic attacks or injury. Click image to continue.
+&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Image Source='../images/Spectre1.gif' Height='275'  Width='550' Name='SpectreMagic'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8523,8 +8523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B489" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B490" sqref="B490"/>
+    <sheetView tabSelected="1" topLeftCell="B241" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B242" sqref="B242:B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8546,7 +8546,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9938,7 +9938,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10458,7 +10458,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>883</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10466,7 +10466,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10474,7 +10474,7 @@
         <v>518</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10482,7 +10482,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10490,7 +10490,7 @@
         <v>561</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10498,7 +10498,7 @@
         <v>562</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10506,7 +10506,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10514,7 +10514,7 @@
         <v>605</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10522,7 +10522,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10530,7 +10530,7 @@
         <v>579</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10538,7 +10538,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10546,7 +10546,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10554,7 +10554,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10562,7 +10562,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10570,7 +10570,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10578,7 +10578,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10586,7 +10586,7 @@
         <v>566</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10594,7 +10594,7 @@
         <v>567</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10602,7 +10602,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10610,7 +10610,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10618,7 +10618,7 @@
         <v>565</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10626,7 +10626,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10634,7 +10634,7 @@
         <v>580</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10642,7 +10642,7 @@
         <v>581</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10650,7 +10650,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10658,7 +10658,7 @@
         <v>582</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10666,7 +10666,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10682,7 +10682,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10690,7 +10690,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10706,7 +10706,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10714,7 +10714,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10730,7 +10730,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10738,7 +10738,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10746,7 +10746,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10762,7 +10762,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10770,7 +10770,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10778,7 +10778,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10786,7 +10786,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10794,7 +10794,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10802,7 +10802,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10810,7 +10810,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10818,7 +10818,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10826,7 +10826,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10834,7 +10834,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10842,7 +10842,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10850,7 +10850,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10858,7 +10858,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10866,7 +10866,7 @@
         <v>593</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10874,7 +10874,7 @@
         <v>592</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10882,7 +10882,7 @@
         <v>594</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10890,7 +10890,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10898,7 +10898,7 @@
         <v>595</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10906,7 +10906,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10914,7 +10914,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10922,7 +10922,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10930,7 +10930,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10938,7 +10938,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10946,7 +10946,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10954,7 +10954,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10962,7 +10962,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10970,7 +10970,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10986,7 +10986,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10994,7 +10994,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11002,7 +11002,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11026,7 +11026,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11034,7 +11034,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11042,7 +11042,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11050,7 +11050,7 @@
         <v>588</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11058,7 +11058,7 @@
         <v>589</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11066,7 +11066,7 @@
         <v>590</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11074,7 +11074,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11082,7 +11082,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11090,7 +11090,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11098,7 +11098,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11106,7 +11106,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11122,7 +11122,7 @@
         <v>412</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11130,7 +11130,7 @@
         <v>413</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11138,7 +11138,7 @@
         <v>414</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11146,7 +11146,7 @@
         <v>415</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11154,7 +11154,7 @@
         <v>416</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11162,7 +11162,7 @@
         <v>601</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11170,7 +11170,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11186,7 +11186,7 @@
         <v>424</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11194,7 +11194,7 @@
         <v>425</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11202,7 +11202,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11210,7 +11210,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11218,7 +11218,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11226,7 +11226,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11234,7 +11234,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11242,7 +11242,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11250,7 +11250,7 @@
         <v>539</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11258,7 +11258,7 @@
         <v>540</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11266,7 +11266,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11274,7 +11274,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11282,7 +11282,7 @@
         <v>385</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11298,7 +11298,7 @@
         <v>610</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11306,7 +11306,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11314,7 +11314,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11330,7 +11330,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11338,7 +11338,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11346,7 +11346,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11362,7 +11362,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11370,7 +11370,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11378,7 +11378,7 @@
         <v>382</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11386,7 +11386,7 @@
         <v>383</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11394,7 +11394,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11402,7 +11402,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11410,7 +11410,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11418,7 +11418,7 @@
         <v>462</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11426,7 +11426,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11442,7 +11442,7 @@
         <v>333</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11450,7 +11450,7 @@
         <v>612</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11458,7 +11458,7 @@
         <v>613</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11466,7 +11466,7 @@
         <v>615</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11474,7 +11474,7 @@
         <v>616</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11482,7 +11482,7 @@
         <v>617</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11490,7 +11490,7 @@
         <v>618</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11498,7 +11498,7 @@
         <v>619</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11506,7 +11506,7 @@
         <v>620</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11514,7 +11514,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11522,7 +11522,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11530,7 +11530,7 @@
         <v>608</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11538,7 +11538,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11546,7 +11546,7 @@
         <v>328</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11554,7 +11554,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11562,7 +11562,7 @@
         <v>484</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11570,7 +11570,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11578,7 +11578,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11586,7 +11586,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11594,7 +11594,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11602,7 +11602,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11610,7 +11610,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11658,7 +11658,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11666,7 +11666,7 @@
         <v>456</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11674,7 +11674,7 @@
         <v>457</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11682,7 +11682,7 @@
         <v>458</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11690,7 +11690,7 @@
         <v>459</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11698,7 +11698,7 @@
         <v>460</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11706,7 +11706,7 @@
         <v>461</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11714,7 +11714,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11786,7 +11786,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11794,7 +11794,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11802,7 +11802,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11810,7 +11810,7 @@
         <v>473</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11818,7 +11818,7 @@
         <v>474</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11826,7 +11826,7 @@
         <v>475</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11834,7 +11834,7 @@
         <v>476</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11842,7 +11842,7 @@
         <v>477</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11850,7 +11850,7 @@
         <v>478</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11858,7 +11858,7 @@
         <v>609</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11866,7 +11866,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11874,7 +11874,7 @@
         <v>466</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11882,7 +11882,7 @@
         <v>467</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11890,7 +11890,7 @@
         <v>468</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11898,7 +11898,7 @@
         <v>469</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11906,7 +11906,7 @@
         <v>470</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11914,7 +11914,7 @@
         <v>471</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11922,7 +11922,7 @@
         <v>472</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11930,7 +11930,7 @@
         <v>607</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11938,7 +11938,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11946,7 +11946,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11954,7 +11954,7 @@
         <v>417</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11962,7 +11962,7 @@
         <v>418</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11970,7 +11970,7 @@
         <v>419</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11978,7 +11978,7 @@
         <v>420</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11986,7 +11986,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11994,7 +11994,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12002,7 +12002,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12010,7 +12010,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12018,7 +12018,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12026,7 +12026,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12034,7 +12034,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12042,7 +12042,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12050,7 +12050,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12058,7 +12058,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12066,7 +12066,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12074,7 +12074,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12082,7 +12082,7 @@
         <v>329</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12090,7 +12090,7 @@
         <v>384</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12098,7 +12098,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12106,7 +12106,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -12114,7 +12114,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12122,7 +12122,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12130,7 +12130,7 @@
         <v>606</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12138,7 +12138,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12146,7 +12146,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12154,7 +12154,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12162,7 +12162,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12170,7 +12170,7 @@
         <v>378</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12178,7 +12178,7 @@
         <v>379</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12186,7 +12186,7 @@
         <v>441</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12202,7 +12202,7 @@
         <v>526</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12250,7 +12250,7 @@
         <v>591</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12258,7 +12258,7 @@
         <v>322</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12266,7 +12266,7 @@
         <v>394</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12274,7 +12274,7 @@
         <v>393</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12282,7 +12282,7 @@
         <v>395</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12290,7 +12290,7 @@
         <v>396</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12298,7 +12298,7 @@
         <v>397</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12306,7 +12306,7 @@
         <v>398</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12314,7 +12314,7 @@
         <v>399</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12322,7 +12322,7 @@
         <v>428</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12330,7 +12330,7 @@
         <v>429</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12338,7 +12338,7 @@
         <v>634</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12346,7 +12346,7 @@
         <v>430</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12354,7 +12354,7 @@
         <v>431</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12362,7 +12362,7 @@
         <v>432</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12370,7 +12370,7 @@
         <v>433</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12378,7 +12378,7 @@
         <v>434</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12386,7 +12386,7 @@
         <v>435</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12394,7 +12394,7 @@
         <v>436</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12402,7 +12402,7 @@
         <v>437</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12410,7 +12410,7 @@
         <v>438</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12418,7 +12418,7 @@
         <v>439</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12426,7 +12426,7 @@
         <v>440</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12434,7 +12434,7 @@
         <v>455</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12442,7 +12442,7 @@
         <v>463</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12450,7 +12450,7 @@
         <v>464</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12458,7 +12458,7 @@
         <v>465</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12466,7 +12466,7 @@
         <v>545</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12474,7 +12474,7 @@
         <v>621</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12482,7 +12482,7 @@
         <v>485</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12490,7 +12490,7 @@
         <v>486</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12498,7 +12498,7 @@
         <v>487</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>488</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12514,7 +12514,7 @@
         <v>489</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12522,7 +12522,7 @@
         <v>490</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12530,7 +12530,7 @@
         <v>491</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12538,7 +12538,7 @@
         <v>492</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12546,7 +12546,7 @@
         <v>493</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12554,7 +12554,7 @@
         <v>494</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12562,7 +12562,7 @@
         <v>495</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12570,7 +12570,7 @@
         <v>496</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12578,7 +12578,7 @@
         <v>497</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12586,7 +12586,7 @@
         <v>498</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12594,7 +12594,7 @@
         <v>499</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12602,7 +12602,7 @@
         <v>586</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12610,7 +12610,7 @@
         <v>587</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12618,7 +12618,7 @@
         <v>500</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12626,7 +12626,7 @@
         <v>512</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12634,7 +12634,7 @@
         <v>421</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12658,7 +12658,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12666,7 +12666,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12674,7 +12674,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12682,7 +12682,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12690,7 +12690,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12698,7 +12698,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12706,7 +12706,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12714,7 +12714,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12722,7 +12722,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12730,7 +12730,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12738,7 +12738,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12818,7 +12818,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12826,7 +12826,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12842,7 +12842,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12850,7 +12850,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12858,7 +12858,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12866,7 +12866,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12914,7 +12914,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12922,7 +12922,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12930,7 +12930,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12938,7 +12938,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12946,7 +12946,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12954,7 +12954,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12962,7 +12962,7 @@
         <v>353</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12970,7 +12970,7 @@
         <v>365</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12978,7 +12978,7 @@
         <v>366</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12986,7 +12986,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12994,7 +12994,7 @@
         <v>364</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -13002,7 +13002,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13010,7 +13010,7 @@
         <v>354</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13026,7 +13026,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13034,7 +13034,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13042,7 +13042,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13050,7 +13050,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13058,7 +13058,7 @@
         <v>363</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13066,7 +13066,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13074,7 +13074,7 @@
         <v>361</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13090,7 +13090,7 @@
         <v>514</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13098,7 +13098,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13106,7 +13106,7 @@
         <v>358</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13114,7 +13114,7 @@
         <v>359</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13130,7 +13130,7 @@
         <v>515</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13138,7 +13138,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13146,7 +13146,7 @@
         <v>352</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13154,7 +13154,7 @@
         <v>355</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13162,7 +13162,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13170,7 +13170,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13194,7 +13194,7 @@
         <v>349</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13202,7 +13202,7 @@
         <v>516</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -13210,7 +13210,7 @@
         <v>326</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13234,7 +13234,7 @@
         <v>651</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13250,7 +13250,7 @@
         <v>652</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempt to fix negative gold problem. Added logging to TransportMgr to help determine if problem still exists. Fix Magican starting attributes. Fix end game stats on number of audiences.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDD1CDB9-CBE7-4195-A9A6-B3385EC2196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1EB1A71-35BB-49AA-A306-D6E73C3705C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2433,12 +2433,6 @@
     <t>e503a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e503a Game Feats &lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You completed an achievement that requires great courage, skill, and persistence.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Congratulations!
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click start to continue.</t>
-  </si>
-  <si>
     <t>e001a</t>
   </si>
   <si>
@@ -8129,6 +8123,12 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You cannot ride away since there are no mounts
  &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Click anywhere to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e503a Game Feats &lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You completed an achievement that requires great courage, skill, and persistence.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Congratulations!
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click star to continue.</t>
   </si>
 </sst>
 </file>
@@ -8523,8 +8523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B527" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B531" sqref="B531"/>
+    <sheetView tabSelected="1" topLeftCell="A382" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B384" sqref="B384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8538,7 +8538,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -8546,7 +8546,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8554,7 +8554,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8562,7 +8562,7 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8570,7 +8570,7 @@
         <v>595</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8578,15 +8578,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8594,7 +8594,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8602,7 +8602,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8610,7 +8610,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8618,7 +8618,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8626,7 +8626,7 @@
         <v>258</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8642,7 +8642,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8650,7 +8650,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8658,7 +8658,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -8666,7 +8666,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8674,7 +8674,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8682,7 +8682,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8690,7 +8690,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8698,7 +8698,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8706,7 +8706,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8714,7 +8714,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8722,7 +8722,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8730,7 +8730,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8738,7 +8738,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -8746,7 +8746,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8754,7 +8754,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8762,7 +8762,7 @@
         <v>261</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8770,7 +8770,7 @@
         <v>545</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8778,7 +8778,7 @@
         <v>546</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8786,7 +8786,7 @@
         <v>548</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8794,7 +8794,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8802,7 +8802,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8810,7 +8810,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8818,7 +8818,7 @@
         <v>550</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8826,7 +8826,7 @@
         <v>551</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8834,7 +8834,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8842,7 +8842,7 @@
         <v>557</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8850,7 +8850,7 @@
         <v>558</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8858,7 +8858,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8866,7 +8866,7 @@
         <v>262</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8874,7 +8874,7 @@
         <v>263</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8882,7 +8882,7 @@
         <v>27</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -8890,7 +8890,7 @@
         <v>28</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -8898,7 +8898,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8906,7 +8906,7 @@
         <v>30</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8914,7 +8914,7 @@
         <v>407</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8922,7 +8922,7 @@
         <v>502</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8930,7 +8930,7 @@
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8938,7 +8938,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8946,7 +8946,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8954,7 +8954,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8962,7 +8962,7 @@
         <v>408</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8970,7 +8970,7 @@
         <v>409</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8978,7 +8978,7 @@
         <v>400</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8986,7 +8986,7 @@
         <v>401</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8994,7 +8994,7 @@
         <v>402</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9002,7 +9002,7 @@
         <v>264</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9010,7 +9010,7 @@
         <v>265</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9018,7 +9018,7 @@
         <v>404</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9026,7 +9026,7 @@
         <v>426</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9034,7 +9034,7 @@
         <v>35</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9042,7 +9042,7 @@
         <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>405</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9058,7 +9058,7 @@
         <v>406</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9066,7 +9066,7 @@
         <v>37</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -9082,7 +9082,7 @@
         <v>43</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9090,7 +9090,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9098,7 +9098,7 @@
         <v>503</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9106,7 +9106,7 @@
         <v>504</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9114,7 +9114,7 @@
         <v>39</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -9122,7 +9122,7 @@
         <v>40</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9130,7 +9130,7 @@
         <v>41</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9138,7 +9138,7 @@
         <v>45</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9146,7 +9146,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9154,7 +9154,7 @@
         <v>46</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9162,7 +9162,7 @@
         <v>47</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9170,7 +9170,7 @@
         <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9178,7 +9178,7 @@
         <v>49</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9186,7 +9186,7 @@
         <v>50</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9194,7 +9194,7 @@
         <v>51</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9202,7 +9202,7 @@
         <v>52</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9210,7 +9210,7 @@
         <v>53</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -9218,7 +9218,7 @@
         <v>54</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9226,7 +9226,7 @@
         <v>55</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9234,7 +9234,7 @@
         <v>56</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9242,7 +9242,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9250,7 +9250,7 @@
         <v>58</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9258,7 +9258,7 @@
         <v>523</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9266,7 +9266,7 @@
         <v>524</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9274,7 +9274,7 @@
         <v>527</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9282,7 +9282,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9290,7 +9290,7 @@
         <v>556</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9298,7 +9298,7 @@
         <v>60</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9306,7 +9306,7 @@
         <v>522</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9314,7 +9314,7 @@
         <v>61</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9322,7 +9322,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9330,7 +9330,7 @@
         <v>341</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9338,7 +9338,7 @@
         <v>63</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -9346,7 +9346,7 @@
         <v>64</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9354,7 +9354,7 @@
         <v>65</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9362,7 +9362,7 @@
         <v>66</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9370,7 +9370,7 @@
         <v>329</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9378,7 +9378,7 @@
         <v>67</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9386,7 +9386,7 @@
         <v>386</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9394,7 +9394,7 @@
         <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9402,7 +9402,7 @@
         <v>342</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9410,7 +9410,7 @@
         <v>387</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9418,7 +9418,7 @@
         <v>69</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9426,7 +9426,7 @@
         <v>390</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9434,7 +9434,7 @@
         <v>391</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9442,7 +9442,7 @@
         <v>70</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -9450,7 +9450,7 @@
         <v>343</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9458,7 +9458,7 @@
         <v>259</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9466,7 +9466,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9474,7 +9474,7 @@
         <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9482,7 +9482,7 @@
         <v>73</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9498,7 +9498,7 @@
         <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9514,7 +9514,7 @@
         <v>324</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9522,7 +9522,7 @@
         <v>621</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9530,7 +9530,7 @@
         <v>76</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9538,7 +9538,7 @@
         <v>77</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9562,7 +9562,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9570,7 +9570,7 @@
         <v>349</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9578,7 +9578,7 @@
         <v>350</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9586,7 +9586,7 @@
         <v>79</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9594,7 +9594,7 @@
         <v>346</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9602,7 +9602,7 @@
         <v>347</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9610,7 +9610,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9618,7 +9618,7 @@
         <v>81</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9626,7 +9626,7 @@
         <v>568</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9634,7 +9634,7 @@
         <v>569</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9642,7 +9642,7 @@
         <v>570</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9650,7 +9650,7 @@
         <v>571</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9658,7 +9658,7 @@
         <v>572</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9666,7 +9666,7 @@
         <v>573</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9674,7 +9674,7 @@
         <v>574</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9682,7 +9682,7 @@
         <v>575</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9690,7 +9690,7 @@
         <v>576</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9698,7 +9698,7 @@
         <v>577</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9706,7 +9706,7 @@
         <v>82</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9714,7 +9714,7 @@
         <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9722,7 +9722,7 @@
         <v>601</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9730,7 +9730,7 @@
         <v>84</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9738,7 +9738,7 @@
         <v>85</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9746,7 +9746,7 @@
         <v>425</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9754,7 +9754,7 @@
         <v>634</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9762,7 +9762,7 @@
         <v>86</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9770,7 +9770,7 @@
         <v>87</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9778,7 +9778,7 @@
         <v>333</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9786,7 +9786,7 @@
         <v>370</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -9794,7 +9794,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9802,7 +9802,7 @@
         <v>334</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9810,7 +9810,7 @@
         <v>335</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9818,7 +9818,7 @@
         <v>336</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9826,7 +9826,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9834,7 +9834,7 @@
         <v>337</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9842,7 +9842,7 @@
         <v>339</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9850,7 +9850,7 @@
         <v>340</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9858,7 +9858,7 @@
         <v>509</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9866,7 +9866,7 @@
         <v>89</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9874,7 +9874,7 @@
         <v>375</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9882,7 +9882,7 @@
         <v>376</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9890,7 +9890,7 @@
         <v>379</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9898,7 +9898,7 @@
         <v>90</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9906,7 +9906,7 @@
         <v>535</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9914,7 +9914,7 @@
         <v>536</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9922,7 +9922,7 @@
         <v>91</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9930,7 +9930,7 @@
         <v>380</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9938,7 +9938,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9946,7 +9946,7 @@
         <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9970,7 +9970,7 @@
         <v>96</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9978,7 +9978,7 @@
         <v>540</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9986,7 +9986,7 @@
         <v>541</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9994,7 +9994,7 @@
         <v>542</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10002,7 +10002,7 @@
         <v>543</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10010,7 +10010,7 @@
         <v>547</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10026,7 +10026,7 @@
         <v>97</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10034,7 +10034,7 @@
         <v>98</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10042,7 +10042,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10050,7 +10050,7 @@
         <v>101</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10058,7 +10058,7 @@
         <v>100</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10066,7 +10066,7 @@
         <v>102</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10074,7 +10074,7 @@
         <v>103</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10082,7 +10082,7 @@
         <v>104</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10090,7 +10090,7 @@
         <v>105</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10098,7 +10098,7 @@
         <v>500</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10106,7 +10106,7 @@
         <v>501</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10114,7 +10114,7 @@
         <v>106</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10122,7 +10122,7 @@
         <v>107</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10130,7 +10130,7 @@
         <v>165</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10138,7 +10138,7 @@
         <v>537</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10146,7 +10146,7 @@
         <v>108</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -10154,7 +10154,7 @@
         <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10162,7 +10162,7 @@
         <v>110</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10170,7 +10170,7 @@
         <v>166</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10178,7 +10178,7 @@
         <v>167</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10186,7 +10186,7 @@
         <v>168</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10194,7 +10194,7 @@
         <v>552</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10210,7 +10210,7 @@
         <v>111</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10218,7 +10218,7 @@
         <v>506</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10226,7 +10226,7 @@
         <v>507</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10242,7 +10242,7 @@
         <v>512</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10250,7 +10250,7 @@
         <v>112</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10258,7 +10258,7 @@
         <v>169</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10266,7 +10266,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10274,7 +10274,7 @@
         <v>171</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10282,7 +10282,7 @@
         <v>113</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10290,7 +10290,7 @@
         <v>114</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10298,7 +10298,7 @@
         <v>266</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10306,7 +10306,7 @@
         <v>559</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10314,7 +10314,7 @@
         <v>115</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10322,7 +10322,7 @@
         <v>518</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10330,7 +10330,7 @@
         <v>116</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10338,7 +10338,7 @@
         <v>516</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10346,7 +10346,7 @@
         <v>117</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10354,7 +10354,7 @@
         <v>519</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10362,7 +10362,7 @@
         <v>520</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10370,7 +10370,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10378,7 +10378,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10386,7 +10386,7 @@
         <v>562</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10394,7 +10394,7 @@
         <v>563</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10402,7 +10402,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10410,7 +10410,7 @@
         <v>555</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10418,7 +10418,7 @@
         <v>554</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10426,7 +10426,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10434,7 +10434,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10442,7 +10442,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10450,7 +10450,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10458,7 +10458,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10466,7 +10466,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10474,7 +10474,7 @@
         <v>517</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10482,7 +10482,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10490,7 +10490,7 @@
         <v>560</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10498,7 +10498,7 @@
         <v>561</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10506,7 +10506,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10514,7 +10514,7 @@
         <v>604</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10522,7 +10522,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10530,7 +10530,7 @@
         <v>578</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10538,7 +10538,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10546,7 +10546,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10554,7 +10554,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10562,7 +10562,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10570,7 +10570,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10578,7 +10578,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10586,7 +10586,7 @@
         <v>565</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10594,7 +10594,7 @@
         <v>566</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10602,7 +10602,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10610,7 +10610,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10618,7 +10618,7 @@
         <v>564</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10626,7 +10626,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10634,7 +10634,7 @@
         <v>579</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10642,7 +10642,7 @@
         <v>580</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10650,7 +10650,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10658,7 +10658,7 @@
         <v>581</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10666,7 +10666,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10682,7 +10682,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10690,7 +10690,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10706,7 +10706,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10714,7 +10714,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10730,7 +10730,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10738,7 +10738,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10746,7 +10746,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10762,7 +10762,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10770,7 +10770,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10778,7 +10778,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10786,7 +10786,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10794,7 +10794,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10802,7 +10802,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10810,7 +10810,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10818,7 +10818,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10826,7 +10826,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10834,7 +10834,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10842,7 +10842,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10850,7 +10850,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10858,7 +10858,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10866,7 +10866,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10874,7 +10874,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10882,7 +10882,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10890,7 +10890,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10898,7 +10898,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10906,7 +10906,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10914,7 +10914,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10922,7 +10922,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10930,7 +10930,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10938,7 +10938,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10946,7 +10946,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10954,7 +10954,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10962,7 +10962,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10970,7 +10970,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10986,7 +10986,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10994,7 +10994,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11002,7 +11002,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11026,7 +11026,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11034,7 +11034,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11042,7 +11042,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11050,7 +11050,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11058,7 +11058,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11066,7 +11066,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11074,7 +11074,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11082,7 +11082,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11090,7 +11090,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11098,7 +11098,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11106,7 +11106,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11122,7 +11122,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11130,7 +11130,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11138,7 +11138,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11146,7 +11146,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11154,7 +11154,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11162,7 +11162,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11170,7 +11170,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11186,7 +11186,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11194,7 +11194,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11202,7 +11202,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11210,7 +11210,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11218,7 +11218,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11226,7 +11226,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11234,7 +11234,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11242,7 +11242,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11250,7 +11250,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11258,7 +11258,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11266,7 +11266,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11274,7 +11274,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11282,7 +11282,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11298,7 +11298,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11306,7 +11306,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11314,7 +11314,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11330,7 +11330,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11338,7 +11338,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11346,7 +11346,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11362,7 +11362,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11370,7 +11370,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11378,7 +11378,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11386,7 +11386,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11394,7 +11394,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11402,7 +11402,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11410,7 +11410,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11418,7 +11418,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11426,7 +11426,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11442,7 +11442,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11450,7 +11450,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11458,7 +11458,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11466,7 +11466,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11474,7 +11474,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11482,7 +11482,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11490,7 +11490,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11498,7 +11498,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11506,7 +11506,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11514,7 +11514,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11522,7 +11522,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11530,7 +11530,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11538,7 +11538,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11546,7 +11546,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11554,7 +11554,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11562,7 +11562,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11570,7 +11570,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11578,7 +11578,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11586,7 +11586,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11594,7 +11594,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11602,7 +11602,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11610,7 +11610,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11658,7 +11658,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11666,7 +11666,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11674,7 +11674,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11682,7 +11682,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11690,7 +11690,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11698,7 +11698,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11706,7 +11706,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11714,7 +11714,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11786,7 +11786,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11794,7 +11794,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11802,7 +11802,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11810,7 +11810,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11818,7 +11818,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11826,7 +11826,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11834,7 +11834,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11842,7 +11842,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11850,7 +11850,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11858,7 +11858,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11866,7 +11866,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11874,7 +11874,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11882,7 +11882,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11890,7 +11890,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11898,7 +11898,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11906,7 +11906,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11914,7 +11914,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11922,7 +11922,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11930,7 +11930,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11938,7 +11938,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11946,7 +11946,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11954,7 +11954,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11962,7 +11962,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11970,7 +11970,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11978,7 +11978,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11986,7 +11986,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11994,7 +11994,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12002,7 +12002,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12010,7 +12010,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12018,7 +12018,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12026,7 +12026,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12034,7 +12034,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12042,7 +12042,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12050,7 +12050,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12058,7 +12058,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12066,7 +12066,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12074,7 +12074,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12082,7 +12082,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12090,7 +12090,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12098,7 +12098,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12106,7 +12106,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -12114,7 +12114,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12122,7 +12122,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12130,7 +12130,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12138,7 +12138,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12146,7 +12146,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12154,7 +12154,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12162,7 +12162,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12170,7 +12170,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12178,7 +12178,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12186,7 +12186,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12202,7 +12202,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12250,7 +12250,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12258,7 +12258,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12266,7 +12266,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12274,7 +12274,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12282,7 +12282,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12290,7 +12290,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12298,7 +12298,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12306,7 +12306,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12314,7 +12314,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12322,7 +12322,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12330,7 +12330,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12338,7 +12338,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12346,7 +12346,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12354,7 +12354,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12362,7 +12362,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12370,7 +12370,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12378,7 +12378,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12386,7 +12386,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12394,7 +12394,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12402,7 +12402,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12410,7 +12410,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12418,7 +12418,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12426,7 +12426,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12434,7 +12434,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12442,7 +12442,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12450,7 +12450,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12458,7 +12458,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12466,7 +12466,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12474,7 +12474,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12482,7 +12482,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12490,7 +12490,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12498,7 +12498,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12514,7 +12514,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12522,7 +12522,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12530,7 +12530,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12538,7 +12538,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12546,7 +12546,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12554,7 +12554,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12562,7 +12562,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12570,7 +12570,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12578,7 +12578,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12586,7 +12586,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12594,7 +12594,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12602,7 +12602,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12610,7 +12610,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12618,7 +12618,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12626,7 +12626,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12634,7 +12634,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12658,7 +12658,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12666,7 +12666,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12674,7 +12674,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12682,7 +12682,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12690,7 +12690,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12698,7 +12698,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12706,7 +12706,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12714,7 +12714,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12722,7 +12722,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12730,7 +12730,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12738,7 +12738,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12770,7 +12770,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12818,7 +12818,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12826,7 +12826,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12842,7 +12842,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12850,7 +12850,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12858,7 +12858,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12866,7 +12866,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12914,7 +12914,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12922,7 +12922,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12930,7 +12930,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12938,7 +12938,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12946,7 +12946,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12954,7 +12954,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12962,7 +12962,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12970,7 +12970,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12978,7 +12978,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12986,7 +12986,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12994,7 +12994,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -13002,7 +13002,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13010,7 +13010,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13026,7 +13026,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13034,7 +13034,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13042,7 +13042,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13050,7 +13050,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13058,7 +13058,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13066,7 +13066,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13074,7 +13074,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13090,7 +13090,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13098,7 +13098,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13106,7 +13106,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13114,7 +13114,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13130,7 +13130,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13138,7 +13138,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13146,7 +13146,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13154,7 +13154,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13162,7 +13162,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13170,7 +13170,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13194,7 +13194,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13202,7 +13202,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -13210,7 +13210,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13234,7 +13234,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13242,7 +13242,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>653</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13250,7 +13250,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing to release new version. Added logging level to show serialization/deseralization of game properties.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1EB1A71-35BB-49AA-A306-D6E73C3705C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01C894B4-AE99-46DB-86B6-FFA0BC322794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -4922,12 +4922,6 @@
                           &lt;InlineUIContainer&gt;&lt;Image Name='EncounterEnd' Source='../images/MountainsView.gif' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e078c Bad Going For Horses&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Terrain is difficult on horses.  If you choose Travel for the daily action tomorrow, you will risk losing horses. Any other activity will nullify this event. Click Image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                          &lt;InlineUIContainer&gt;&lt;Image Name='MountainPath' Source='../images/MountainPath.gif' Height='258' Width='280'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e079 Heavy Rains&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Cold, driving rains hinder man and beast. You must stop moving today. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die for each character in your party. If the result is a 5 plus, the character catches a cold and suffers one wound.
@@ -8129,6 +8123,12 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You completed an achievement that requires great courage, skill, and persistence.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Congratulations!
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Click star to continue.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e078c Bad Going For Horses&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Terrain is difficult on horses.  If you choose Travel for the daily action tomorrow, you will risk losing horses. Any other activity will nullify this event. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                          &lt;InlineUIContainer&gt;&lt;Image Name='MountainPath' Source='../images/MountainPath.gif' Height='258' Width='280'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8523,8 +8523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B384" sqref="B384"/>
+    <sheetView tabSelected="1" topLeftCell="B227" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8546,7 +8546,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9938,7 +9938,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10370,7 +10370,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>870</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10378,7 +10378,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10386,7 +10386,7 @@
         <v>562</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10394,7 +10394,7 @@
         <v>563</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10402,7 +10402,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10410,7 +10410,7 @@
         <v>555</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10418,7 +10418,7 @@
         <v>554</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10426,7 +10426,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10434,7 +10434,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10442,7 +10442,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10450,7 +10450,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10458,7 +10458,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10466,7 +10466,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10474,7 +10474,7 @@
         <v>517</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10482,7 +10482,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10490,7 +10490,7 @@
         <v>560</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10498,7 +10498,7 @@
         <v>561</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10506,7 +10506,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10514,7 +10514,7 @@
         <v>604</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10522,7 +10522,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10530,7 +10530,7 @@
         <v>578</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10538,7 +10538,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10546,7 +10546,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10554,7 +10554,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10562,7 +10562,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10570,7 +10570,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10578,7 +10578,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10586,7 +10586,7 @@
         <v>565</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10594,7 +10594,7 @@
         <v>566</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10602,7 +10602,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10610,7 +10610,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10618,7 +10618,7 @@
         <v>564</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10626,7 +10626,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10634,7 +10634,7 @@
         <v>579</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10642,7 +10642,7 @@
         <v>580</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10650,7 +10650,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10658,7 +10658,7 @@
         <v>581</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10666,7 +10666,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10674,7 +10674,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10682,7 +10682,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10690,7 +10690,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10706,7 +10706,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10714,7 +10714,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10730,7 +10730,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10738,7 +10738,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10746,7 +10746,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10762,7 +10762,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10770,7 +10770,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10778,7 +10778,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10786,7 +10786,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10794,7 +10794,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10802,7 +10802,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10810,7 +10810,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10818,7 +10818,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10826,7 +10826,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10834,7 +10834,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10842,7 +10842,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10850,7 +10850,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10858,7 +10858,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10866,7 +10866,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10874,7 +10874,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10882,7 +10882,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10890,7 +10890,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10898,7 +10898,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10906,7 +10906,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10914,7 +10914,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10922,7 +10922,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10930,7 +10930,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10938,7 +10938,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10946,7 +10946,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10954,7 +10954,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10962,7 +10962,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10970,7 +10970,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10986,7 +10986,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10994,7 +10994,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11002,7 +11002,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11018,7 +11018,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11026,7 +11026,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11034,7 +11034,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11042,7 +11042,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11050,7 +11050,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11058,7 +11058,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11066,7 +11066,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11074,7 +11074,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11082,7 +11082,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11090,7 +11090,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11098,7 +11098,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11106,7 +11106,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11122,7 +11122,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11130,7 +11130,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11138,7 +11138,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11146,7 +11146,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11154,7 +11154,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11162,7 +11162,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11170,7 +11170,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11186,7 +11186,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11194,7 +11194,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11202,7 +11202,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11210,7 +11210,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11218,7 +11218,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11226,7 +11226,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11234,7 +11234,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11242,7 +11242,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11250,7 +11250,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11258,7 +11258,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11266,7 +11266,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11274,7 +11274,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11282,7 +11282,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11298,7 +11298,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11306,7 +11306,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11314,7 +11314,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11330,7 +11330,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11338,7 +11338,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11346,7 +11346,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11362,7 +11362,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11370,7 +11370,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11378,7 +11378,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11386,7 +11386,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11394,7 +11394,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11402,7 +11402,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11410,7 +11410,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11418,7 +11418,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11426,7 +11426,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11442,7 +11442,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11450,7 +11450,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11458,7 +11458,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11466,7 +11466,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11474,7 +11474,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11482,7 +11482,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11490,7 +11490,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11498,7 +11498,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11506,7 +11506,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11514,7 +11514,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11522,7 +11522,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11530,7 +11530,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11538,7 +11538,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11546,7 +11546,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11554,7 +11554,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11562,7 +11562,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11570,7 +11570,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11578,7 +11578,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11586,7 +11586,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11594,7 +11594,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11602,7 +11602,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11610,7 +11610,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11658,7 +11658,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11666,7 +11666,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11674,7 +11674,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11682,7 +11682,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11690,7 +11690,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11698,7 +11698,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11706,7 +11706,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11714,7 +11714,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11786,7 +11786,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11794,7 +11794,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11802,7 +11802,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11810,7 +11810,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11818,7 +11818,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11826,7 +11826,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11834,7 +11834,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11842,7 +11842,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11850,7 +11850,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11858,7 +11858,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11866,7 +11866,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11874,7 +11874,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11882,7 +11882,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11890,7 +11890,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11898,7 +11898,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11906,7 +11906,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11914,7 +11914,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11922,7 +11922,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11930,7 +11930,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11938,7 +11938,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11946,7 +11946,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11954,7 +11954,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11962,7 +11962,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11970,7 +11970,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11978,7 +11978,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11986,7 +11986,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11994,7 +11994,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12002,7 +12002,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12010,7 +12010,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12018,7 +12018,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12026,7 +12026,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12034,7 +12034,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12042,7 +12042,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12050,7 +12050,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12058,7 +12058,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12066,7 +12066,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12074,7 +12074,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12082,7 +12082,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12090,7 +12090,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12098,7 +12098,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12106,7 +12106,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -12114,7 +12114,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12122,7 +12122,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12130,7 +12130,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12138,7 +12138,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12146,7 +12146,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12154,7 +12154,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12162,7 +12162,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12170,7 +12170,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12178,7 +12178,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12186,7 +12186,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12202,7 +12202,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12250,7 +12250,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12258,7 +12258,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12266,7 +12266,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12274,7 +12274,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12282,7 +12282,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12290,7 +12290,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12298,7 +12298,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12306,7 +12306,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12314,7 +12314,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12322,7 +12322,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12330,7 +12330,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12338,7 +12338,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12346,7 +12346,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12354,7 +12354,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12362,7 +12362,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12370,7 +12370,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12378,7 +12378,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12386,7 +12386,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12394,7 +12394,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12402,7 +12402,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12410,7 +12410,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12418,7 +12418,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12426,7 +12426,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12434,7 +12434,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12442,7 +12442,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12450,7 +12450,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12458,7 +12458,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12466,7 +12466,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12474,7 +12474,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12482,7 +12482,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12490,7 +12490,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12498,7 +12498,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12514,7 +12514,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12522,7 +12522,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12530,7 +12530,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12538,7 +12538,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12546,7 +12546,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12554,7 +12554,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12562,7 +12562,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12570,7 +12570,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12578,7 +12578,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12586,7 +12586,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12594,7 +12594,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12602,7 +12602,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12610,7 +12610,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12618,7 +12618,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12626,7 +12626,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12634,7 +12634,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12658,7 +12658,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12666,7 +12666,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12674,7 +12674,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12682,7 +12682,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12690,7 +12690,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12698,7 +12698,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12706,7 +12706,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12714,7 +12714,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12722,7 +12722,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12730,7 +12730,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12738,7 +12738,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12770,7 +12770,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12818,7 +12818,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12826,7 +12826,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12842,7 +12842,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12850,7 +12850,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12858,7 +12858,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12866,7 +12866,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12914,7 +12914,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12922,7 +12922,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12930,7 +12930,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12938,7 +12938,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12946,7 +12946,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12954,7 +12954,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12962,7 +12962,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12970,7 +12970,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12978,7 +12978,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12986,7 +12986,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12994,7 +12994,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -13002,7 +13002,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13010,7 +13010,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13026,7 +13026,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13034,7 +13034,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13042,7 +13042,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13050,7 +13050,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13058,7 +13058,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13066,7 +13066,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13074,7 +13074,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13090,7 +13090,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13098,7 +13098,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13106,7 +13106,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13114,7 +13114,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13130,7 +13130,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13138,7 +13138,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13146,7 +13146,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13154,7 +13154,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13162,7 +13162,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13170,7 +13170,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13194,7 +13194,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13202,7 +13202,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -13210,7 +13210,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13234,7 +13234,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13242,7 +13242,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13250,7 +13250,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix original game win. Fix issue with showing Feats Dialog when feat is shown.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01C894B4-AE99-46DB-86B6-FFA0BC322794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B2FF576-7BB2-4156-AEBF-60B628B5589F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2436,20 +2436,6 @@
     <t>e001a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e001 The Adventure Begins&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Evil events have overtaken your Northlands Kingdom. Your father, the old king, is dead - assassinated by rivals to the throne.  These usurpers now hold the place with their mercenary royal guard. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You have escaped, and must collect 500 gold pieces to raise a force to smash them and retake your heritage. Furthermore, the usurpers have powerful friends overseas. If you can't return to take them out in ten weeks, their allies will arrive and you lose your kingdom forever. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-At dawn, you roll out of the merchant wagons into a ditch, dust off your clothes, loosen your swordbelt, and get ready to start the first day of your adventure &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The original game is brutally difficult to win. The &lt;Bold&gt;recommended&lt;/Bold&gt; fun game provides a random starting party, a random starting hex, food, and coins. Details can be viewed on the &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu where other game options can be selected. If you choose different options, you must select &lt;Bold&gt;File | New&lt;/Bold&gt; menu to start a new game with those options.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='Original Game' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-    or    
-&lt;InlineUIContainer&gt;&lt;Button Content=' Fun Options ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e000d Manual Wits and Wiles&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If you have played the game before and won, you may wish an extra challenge by using a wits and wiles rating one less than the previous value; if you lost in the previous game, use a wit and wiles one higher than the previous value.  
@@ -8129,6 +8115,21 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Terrain is difficult on horses.  If you choose Travel for the daily action tomorrow, you will risk losing horses. Any other activity will nullify this event. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                           &lt;InlineUIContainer&gt;&lt;Image Name='MountainPath' Source='../images/MountainPath.gif' Height='258' Width='280'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e001 The Adventure Begins&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Evil events have overtaken your Northlands Kingdom. Your father, the old king, is dead - assassinated by rivals to the throne.  These usurpers now hold the place with their mercenary royal guard. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You have escaped, and must collect 500 gold pieces to raise a force to smash them and retake your heritage. Furthermore, the usurpers have powerful friends overseas. If you can't return to take them out in ten weeks, their allies will arrive and you lose your kingdom forever. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At dawn, you roll out of the merchant wagons into a ditch, dust off your clothes, loosen your swordbelt, and get ready to start the first day of your adventure &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The original game is brutally difficult to win. The &lt;Bold&gt;recommended&lt;/Bold&gt; fun game provides a random starting party, a random starting hex, food, and coins. Details can be viewed on the &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu where other game options can be selected. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you want different options, you must open the Options Dialog with &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu, and check the &lt;Bold&gt;AutoSetup&lt;/Bold&gt; checkbox. Then, select &lt;Bold&gt;File | New&lt;/Bold&gt; menu to start a new game with those options.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Original Game' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+    or    
+&lt;InlineUIContainer&gt;&lt;Button Content=' Fun Options ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8523,8 +8524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B227" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B231" sqref="B231"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8538,7 +8539,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -8546,7 +8547,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8554,7 +8555,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8562,7 +8563,7 @@
         <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8570,15 +8571,15 @@
         <v>595</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>654</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8586,7 +8587,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8594,7 +8595,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8602,7 +8603,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8610,7 +8611,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8618,7 +8619,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8626,7 +8627,7 @@
         <v>258</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8642,7 +8643,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8650,7 +8651,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8658,7 +8659,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -8666,7 +8667,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8674,7 +8675,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8682,7 +8683,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8690,7 +8691,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8698,7 +8699,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8706,7 +8707,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8714,7 +8715,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8722,7 +8723,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8730,7 +8731,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8738,7 +8739,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -8746,7 +8747,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8754,7 +8755,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8762,7 +8763,7 @@
         <v>261</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8770,7 +8771,7 @@
         <v>545</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -8778,7 +8779,7 @@
         <v>546</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8786,7 +8787,7 @@
         <v>548</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8794,7 +8795,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8802,7 +8803,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8810,7 +8811,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8818,7 +8819,7 @@
         <v>550</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -8826,7 +8827,7 @@
         <v>551</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8834,7 +8835,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -8842,7 +8843,7 @@
         <v>557</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8850,7 +8851,7 @@
         <v>558</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -8858,7 +8859,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8866,7 +8867,7 @@
         <v>262</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -8874,7 +8875,7 @@
         <v>263</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8882,7 +8883,7 @@
         <v>27</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -8890,7 +8891,7 @@
         <v>28</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -8898,7 +8899,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8906,7 +8907,7 @@
         <v>30</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8914,7 +8915,7 @@
         <v>407</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8922,7 +8923,7 @@
         <v>502</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8930,7 +8931,7 @@
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8938,7 +8939,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -8946,7 +8947,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8954,7 +8955,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8962,7 +8963,7 @@
         <v>408</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -8970,7 +8971,7 @@
         <v>409</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8978,7 +8979,7 @@
         <v>400</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -8986,7 +8987,7 @@
         <v>401</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -8994,7 +8995,7 @@
         <v>402</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9002,7 +9003,7 @@
         <v>264</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9010,7 +9011,7 @@
         <v>265</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9018,7 +9019,7 @@
         <v>404</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9026,7 +9027,7 @@
         <v>426</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9034,7 +9035,7 @@
         <v>35</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9042,7 +9043,7 @@
         <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9050,7 +9051,7 @@
         <v>405</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9058,7 +9059,7 @@
         <v>406</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9066,7 +9067,7 @@
         <v>37</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -9082,7 +9083,7 @@
         <v>43</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9090,7 +9091,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9098,7 +9099,7 @@
         <v>503</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9106,7 +9107,7 @@
         <v>504</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9114,7 +9115,7 @@
         <v>39</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -9122,7 +9123,7 @@
         <v>40</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9130,7 +9131,7 @@
         <v>41</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9138,7 +9139,7 @@
         <v>45</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9146,7 +9147,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9154,7 +9155,7 @@
         <v>46</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9162,7 +9163,7 @@
         <v>47</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9170,7 +9171,7 @@
         <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9178,7 +9179,7 @@
         <v>49</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9186,7 +9187,7 @@
         <v>50</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9194,7 +9195,7 @@
         <v>51</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9202,7 +9203,7 @@
         <v>52</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9210,7 +9211,7 @@
         <v>53</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -9218,7 +9219,7 @@
         <v>54</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9226,7 +9227,7 @@
         <v>55</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9234,7 +9235,7 @@
         <v>56</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9242,7 +9243,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9250,7 +9251,7 @@
         <v>58</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9258,7 +9259,7 @@
         <v>523</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9266,7 +9267,7 @@
         <v>524</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9274,7 +9275,7 @@
         <v>527</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9282,7 +9283,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9290,7 +9291,7 @@
         <v>556</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9298,7 +9299,7 @@
         <v>60</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9306,7 +9307,7 @@
         <v>522</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9314,7 +9315,7 @@
         <v>61</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9322,7 +9323,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9330,7 +9331,7 @@
         <v>341</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9338,7 +9339,7 @@
         <v>63</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -9346,7 +9347,7 @@
         <v>64</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9354,7 +9355,7 @@
         <v>65</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9362,7 +9363,7 @@
         <v>66</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9370,7 +9371,7 @@
         <v>329</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9378,7 +9379,7 @@
         <v>67</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9386,7 +9387,7 @@
         <v>386</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9394,7 +9395,7 @@
         <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9402,7 +9403,7 @@
         <v>342</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9410,7 +9411,7 @@
         <v>387</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9418,7 +9419,7 @@
         <v>69</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9426,7 +9427,7 @@
         <v>390</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9434,7 +9435,7 @@
         <v>391</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9442,7 +9443,7 @@
         <v>70</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -9450,7 +9451,7 @@
         <v>343</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9458,7 +9459,7 @@
         <v>259</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9466,7 +9467,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9474,7 +9475,7 @@
         <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9482,7 +9483,7 @@
         <v>73</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9498,7 +9499,7 @@
         <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9514,7 +9515,7 @@
         <v>324</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9522,7 +9523,7 @@
         <v>621</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9530,7 +9531,7 @@
         <v>76</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9538,7 +9539,7 @@
         <v>77</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9562,7 +9563,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9570,7 +9571,7 @@
         <v>349</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9578,7 +9579,7 @@
         <v>350</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9586,7 +9587,7 @@
         <v>79</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9594,7 +9595,7 @@
         <v>346</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9602,7 +9603,7 @@
         <v>347</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9610,7 +9611,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9618,7 +9619,7 @@
         <v>81</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9626,7 +9627,7 @@
         <v>568</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9634,7 +9635,7 @@
         <v>569</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9642,7 +9643,7 @@
         <v>570</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9650,7 +9651,7 @@
         <v>571</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9658,7 +9659,7 @@
         <v>572</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9666,7 +9667,7 @@
         <v>573</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9674,7 +9675,7 @@
         <v>574</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9682,7 +9683,7 @@
         <v>575</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9690,7 +9691,7 @@
         <v>576</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9698,7 +9699,7 @@
         <v>577</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9706,7 +9707,7 @@
         <v>82</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9714,7 +9715,7 @@
         <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -9722,7 +9723,7 @@
         <v>601</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -9730,7 +9731,7 @@
         <v>84</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9738,7 +9739,7 @@
         <v>85</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9746,7 +9747,7 @@
         <v>425</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9754,7 +9755,7 @@
         <v>634</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9762,7 +9763,7 @@
         <v>86</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9770,7 +9771,7 @@
         <v>87</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9778,7 +9779,7 @@
         <v>333</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9786,7 +9787,7 @@
         <v>370</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="345" x14ac:dyDescent="0.25">
@@ -9794,7 +9795,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9802,7 +9803,7 @@
         <v>334</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9810,7 +9811,7 @@
         <v>335</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9818,7 +9819,7 @@
         <v>336</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9826,7 +9827,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9834,7 +9835,7 @@
         <v>337</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9842,7 +9843,7 @@
         <v>339</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9850,7 +9851,7 @@
         <v>340</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9858,7 +9859,7 @@
         <v>509</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9866,7 +9867,7 @@
         <v>89</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9874,7 +9875,7 @@
         <v>375</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9882,7 +9883,7 @@
         <v>376</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -9890,7 +9891,7 @@
         <v>379</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -9898,7 +9899,7 @@
         <v>90</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -9906,7 +9907,7 @@
         <v>535</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9914,7 +9915,7 @@
         <v>536</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -9922,7 +9923,7 @@
         <v>91</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9930,7 +9931,7 @@
         <v>380</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9938,7 +9939,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -9946,7 +9947,7 @@
         <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -9970,7 +9971,7 @@
         <v>96</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -9978,7 +9979,7 @@
         <v>540</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -9986,7 +9987,7 @@
         <v>541</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -9994,7 +9995,7 @@
         <v>542</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10002,7 +10003,7 @@
         <v>543</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10010,7 +10011,7 @@
         <v>547</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10026,7 +10027,7 @@
         <v>97</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10034,7 +10035,7 @@
         <v>98</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10042,7 +10043,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10050,7 +10051,7 @@
         <v>101</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10058,7 +10059,7 @@
         <v>100</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10066,7 +10067,7 @@
         <v>102</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10074,7 +10075,7 @@
         <v>103</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10082,7 +10083,7 @@
         <v>104</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10090,7 +10091,7 @@
         <v>105</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10098,7 +10099,7 @@
         <v>500</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10106,7 +10107,7 @@
         <v>501</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10114,7 +10115,7 @@
         <v>106</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10122,7 +10123,7 @@
         <v>107</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10130,7 +10131,7 @@
         <v>165</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10138,7 +10139,7 @@
         <v>537</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10146,7 +10147,7 @@
         <v>108</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -10154,7 +10155,7 @@
         <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10162,7 +10163,7 @@
         <v>110</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10170,7 +10171,7 @@
         <v>166</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10178,7 +10179,7 @@
         <v>167</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10186,7 +10187,7 @@
         <v>168</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10194,7 +10195,7 @@
         <v>552</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10210,7 +10211,7 @@
         <v>111</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10218,7 +10219,7 @@
         <v>506</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10226,7 +10227,7 @@
         <v>507</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10242,7 +10243,7 @@
         <v>512</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10250,7 +10251,7 @@
         <v>112</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10258,7 +10259,7 @@
         <v>169</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10266,7 +10267,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10274,7 +10275,7 @@
         <v>171</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10282,7 +10283,7 @@
         <v>113</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10290,7 +10291,7 @@
         <v>114</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10298,7 +10299,7 @@
         <v>266</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10306,7 +10307,7 @@
         <v>559</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10314,7 +10315,7 @@
         <v>115</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10322,7 +10323,7 @@
         <v>518</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10330,7 +10331,7 @@
         <v>116</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10338,7 +10339,7 @@
         <v>516</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10346,7 +10347,7 @@
         <v>117</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10354,7 +10355,7 @@
         <v>519</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10362,7 +10363,7 @@
         <v>520</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10370,7 +10371,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10378,7 +10379,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10386,7 +10387,7 @@
         <v>562</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10394,7 +10395,7 @@
         <v>563</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10402,7 +10403,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10410,7 +10411,7 @@
         <v>555</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10418,7 +10419,7 @@
         <v>554</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10426,7 +10427,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10434,7 +10435,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10442,7 +10443,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10450,7 +10451,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10458,7 +10459,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10466,7 +10467,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10474,7 +10475,7 @@
         <v>517</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10482,7 +10483,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10490,7 +10491,7 @@
         <v>560</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10498,7 +10499,7 @@
         <v>561</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10506,7 +10507,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10514,7 +10515,7 @@
         <v>604</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10522,7 +10523,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10530,7 +10531,7 @@
         <v>578</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10538,7 +10539,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10546,7 +10547,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10554,7 +10555,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10562,7 +10563,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10570,7 +10571,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10578,7 +10579,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10586,7 +10587,7 @@
         <v>565</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10594,7 +10595,7 @@
         <v>566</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10602,7 +10603,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10610,7 +10611,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10618,7 +10619,7 @@
         <v>564</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -10626,7 +10627,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10634,7 +10635,7 @@
         <v>579</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10642,7 +10643,7 @@
         <v>580</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10650,7 +10651,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -10658,7 +10659,7 @@
         <v>581</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10666,7 +10667,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -10674,7 +10675,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10682,7 +10683,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10690,7 +10691,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -10706,7 +10707,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10714,7 +10715,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10730,7 +10731,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10738,7 +10739,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10746,7 +10747,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10762,7 +10763,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10770,7 +10771,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10778,7 +10779,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10786,7 +10787,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10794,7 +10795,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10802,7 +10803,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -10810,7 +10811,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10818,7 +10819,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10826,7 +10827,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10834,7 +10835,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10842,7 +10843,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10850,7 +10851,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10858,7 +10859,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10866,7 +10867,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10874,7 +10875,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10882,7 +10883,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10890,7 +10891,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10898,7 +10899,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -10906,7 +10907,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10914,7 +10915,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10922,7 +10923,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10930,7 +10931,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10938,7 +10939,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10946,7 +10947,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10954,7 +10955,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -10962,7 +10963,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10970,7 +10971,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -10986,7 +10987,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10994,7 +10995,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11002,7 +11003,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11018,7 +11019,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11026,7 +11027,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11034,7 +11035,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11042,7 +11043,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11050,7 +11051,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11058,7 +11059,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11066,7 +11067,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11074,7 +11075,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11082,7 +11083,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11090,7 +11091,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11098,7 +11099,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11106,7 +11107,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11122,7 +11123,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11130,7 +11131,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11138,7 +11139,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11146,7 +11147,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11154,7 +11155,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11162,7 +11163,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -11170,7 +11171,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11186,7 +11187,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11194,7 +11195,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="315" x14ac:dyDescent="0.25">
@@ -11202,7 +11203,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11210,7 +11211,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11218,7 +11219,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11226,7 +11227,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11234,7 +11235,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11242,7 +11243,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11250,7 +11251,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11258,7 +11259,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11266,7 +11267,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11274,7 +11275,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11282,7 +11283,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11298,7 +11299,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11306,7 +11307,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11314,7 +11315,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11330,7 +11331,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11338,7 +11339,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11346,7 +11347,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11362,7 +11363,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11370,7 +11371,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11378,7 +11379,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11386,7 +11387,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11394,7 +11395,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11402,7 +11403,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11410,7 +11411,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11418,7 +11419,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -11426,7 +11427,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11442,7 +11443,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11450,7 +11451,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11458,7 +11459,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11466,7 +11467,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11474,7 +11475,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11482,7 +11483,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11490,7 +11491,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11498,7 +11499,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11506,7 +11507,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11514,7 +11515,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11522,7 +11523,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11530,7 +11531,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11538,7 +11539,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11546,7 +11547,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11554,7 +11555,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11562,7 +11563,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11570,7 +11571,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11578,7 +11579,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11586,7 +11587,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11594,7 +11595,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11602,7 +11603,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11610,7 +11611,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11658,7 +11659,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11666,7 +11667,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11674,7 +11675,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11682,7 +11683,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11690,7 +11691,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -11698,7 +11699,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11706,7 +11707,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11714,7 +11715,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -11786,7 +11787,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -11794,7 +11795,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11802,7 +11803,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11810,7 +11811,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11818,7 +11819,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11826,7 +11827,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11834,7 +11835,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11842,7 +11843,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11850,7 +11851,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -11858,7 +11859,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -11866,7 +11867,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11874,7 +11875,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11882,7 +11883,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11890,7 +11891,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11898,7 +11899,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11906,7 +11907,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11914,7 +11915,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11922,7 +11923,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -11930,7 +11931,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -11938,7 +11939,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -11946,7 +11947,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -11954,7 +11955,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11962,7 +11963,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11970,7 +11971,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -11978,7 +11979,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -11986,7 +11987,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11994,7 +11995,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12002,7 +12003,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12010,7 +12011,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12018,7 +12019,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12026,7 +12027,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12034,7 +12035,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12042,7 +12043,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12050,7 +12051,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12058,7 +12059,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12066,7 +12067,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12074,7 +12075,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12082,7 +12083,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12090,7 +12091,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12098,7 +12099,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12106,7 +12107,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -12114,7 +12115,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12122,7 +12123,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12130,7 +12131,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12138,7 +12139,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12146,7 +12147,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12154,7 +12155,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12162,7 +12163,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12170,7 +12171,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12178,7 +12179,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12186,7 +12187,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12202,7 +12203,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12250,7 +12251,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12258,7 +12259,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12266,7 +12267,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12274,7 +12275,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12282,7 +12283,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12290,7 +12291,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12298,7 +12299,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12306,7 +12307,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12314,7 +12315,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12322,7 +12323,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12330,7 +12331,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12338,7 +12339,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12346,7 +12347,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12354,7 +12355,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12362,7 +12363,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12370,7 +12371,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12378,7 +12379,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12386,7 +12387,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12394,7 +12395,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12402,7 +12403,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12410,7 +12411,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12418,7 +12419,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12426,7 +12427,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12434,7 +12435,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12442,7 +12443,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12450,7 +12451,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12458,7 +12459,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12466,7 +12467,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12474,7 +12475,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12482,7 +12483,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12490,7 +12491,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12498,7 +12499,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12506,7 +12507,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12514,7 +12515,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12522,7 +12523,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12530,7 +12531,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12538,7 +12539,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12546,7 +12547,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12554,7 +12555,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12562,7 +12563,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12570,7 +12571,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12578,7 +12579,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12586,7 +12587,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12594,7 +12595,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12602,7 +12603,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12610,7 +12611,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12618,7 +12619,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12626,7 +12627,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12634,7 +12635,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12658,7 +12659,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12666,7 +12667,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12674,7 +12675,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12682,7 +12683,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12690,7 +12691,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12698,7 +12699,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12706,7 +12707,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12714,7 +12715,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12722,7 +12723,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12730,7 +12731,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12738,7 +12739,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12770,7 +12771,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12818,7 +12819,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12826,7 +12827,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12842,7 +12843,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12850,7 +12851,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12858,7 +12859,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12866,7 +12867,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12914,7 +12915,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12922,7 +12923,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12930,7 +12931,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12938,7 +12939,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12946,7 +12947,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12954,7 +12955,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12962,7 +12963,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12970,7 +12971,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12978,7 +12979,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12986,7 +12987,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12994,7 +12995,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -13002,7 +13003,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13010,7 +13011,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13026,7 +13027,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13034,7 +13035,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13042,7 +13043,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13050,7 +13051,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13058,7 +13059,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13066,7 +13067,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13074,7 +13075,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13090,7 +13091,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13098,7 +13099,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13106,7 +13107,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13114,7 +13115,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13130,7 +13131,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13138,7 +13139,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13146,7 +13147,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13154,7 +13155,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13162,7 +13163,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13170,7 +13171,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13194,7 +13195,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13202,7 +13203,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -13210,7 +13211,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13234,7 +13235,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13242,7 +13243,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13250,7 +13251,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with Lady A. secret not rolling twice
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C3DD060-1166-455C-BF8E-BDA986EA2D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{070D18ED-53C0-497D-9751-5395ADA05AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -6599,21 +6599,6 @@
                                         &lt;InlineUIContainer&gt;&lt;Image Source='../images/LadyAeravir.gif' Name='LadyAeravirSupport' Height='350' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e160g Audience with Lady Aeravir Knowing Her Secret&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You are allowed a semi-private interview with the ruler of Aeravir Castle. Since you know her secret, see  &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. You roll twice and pick the result you want.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160a' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 - Shows No Interest&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160b' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 -Distracted &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 - Shows Pity&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160d' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 - Finds Virtue &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160e' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 - Seduction&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='e160f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 - Shows Support
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll die:
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll1' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e161 Audience with Count Drogat&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You are allowed a semi-private interview with the ruler of Drogat Castle. Roll one die for the result and add one if you have a troll skin giving it to the Count. Die Roll = 
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -7269,22 +7254,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Dismiss' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; a random magic user from party to add one to die roll.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll two die and consult list for results:  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r211e Seeking an Audience with Lady Aeravir&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Lady Aeravir. Roll two die and consult the list below for results: 
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e060' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 2 You insult the Lady's dignity and are arrested&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e159' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 You must purify yourself first&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e158' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Untoward remark makes the guards hostile&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 Must learn better court manners&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e153' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 6 Meet the Master of the Household&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e160' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 7 Gain audience if have griffon claw&lt;LineBreak/&gt;
-           8 Audience refused today. You may try again Tomorrow&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Seneschal requires a bribe&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e160' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10 and 12plus - Audience granted&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 11 Meet daughter of the Lady Aeravir&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e211f Seeking an Audience with the Dwarven King&lt;/Bold&gt;
@@ -8131,6 +8100,37 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Start of a new day! Select action button from the Daily Actions panel. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;After all actions, events, food, and lodging are resolved, the day ends. This continues until the end of the 10th week, which ends the game.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;                &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sun3.gif' Height='220'  Width='440'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e211e Seeking an Audience with Lady Aeravir&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Lady Aeravir. Roll two die and consult the list below for results: 
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e060' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 2 You insult the Lady's dignity and are arrested&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e159' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 You must purify yourself first&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e158' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 Untoward remark makes the guards hostile&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e149' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 Must learn better court manners&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e153' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 6 Meet the Master of the Household&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e160' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 7 Gain audience if have griffon claw&lt;LineBreak/&gt;
+           8 Audience refused today. You may try again Tomorrow&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e148' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 9 Seneschal requires a bribe&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e160' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 10 and 12plus - Audience granted&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Content='e154' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 11 Meet daughter of the Lady Aeravir&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e160g Audience with Lady Aeravir Knowing Her Secret&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You are allowed a semi-private interview with the ruler of Aeravir Castle. Since you know her secret, see  &lt;InlineUIContainer&gt;&lt;Button Content='e145' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160a' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 - Shows No Interest&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160b' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 - Distracted &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160c' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 - Shows Pity&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160d' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 4 - Finds Virtue &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160e' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 - Seduction&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='e160f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 - Shows Support
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll die:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll1' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8525,8 +8525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A453" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B454" sqref="B454"/>
+    <sheetView tabSelected="1" topLeftCell="B415" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B416" sqref="B416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8548,7 +8548,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -8580,7 +8580,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9940,7 +9940,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10372,7 +10372,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10460,7 +10460,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10468,7 +10468,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11860,7 +11860,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1028</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11868,7 +11868,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11876,7 +11876,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11884,7 +11884,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11892,7 +11892,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11900,7 +11900,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11908,7 +11908,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11916,7 +11916,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11924,7 +11924,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11932,7 +11932,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11940,7 +11940,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11948,7 +11948,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="288" x14ac:dyDescent="0.3">
@@ -11956,7 +11956,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11964,7 +11964,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11972,7 +11972,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11980,7 +11980,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11988,7 +11988,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -11996,7 +11996,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12004,7 +12004,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12012,7 +12012,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12020,7 +12020,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12028,7 +12028,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12036,7 +12036,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12044,7 +12044,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12052,7 +12052,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12060,7 +12060,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12068,7 +12068,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12076,7 +12076,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12084,7 +12084,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12092,7 +12092,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12100,7 +12100,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12108,7 +12108,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -12116,7 +12116,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12124,7 +12124,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12132,7 +12132,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12140,7 +12140,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12148,7 +12148,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -12156,7 +12156,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12164,7 +12164,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12172,7 +12172,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12180,7 +12180,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12188,7 +12188,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12204,7 +12204,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -12252,7 +12252,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12260,7 +12260,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12268,7 +12268,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12276,7 +12276,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12284,7 +12284,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12292,7 +12292,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12300,7 +12300,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12308,7 +12308,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12316,7 +12316,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12324,7 +12324,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -12332,7 +12332,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12340,7 +12340,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -12348,7 +12348,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12356,7 +12356,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12364,7 +12364,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12372,7 +12372,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12380,7 +12380,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12388,7 +12388,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12396,7 +12396,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12404,7 +12404,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12412,7 +12412,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -12420,7 +12420,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -12428,7 +12428,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12436,7 +12436,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12444,7 +12444,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12452,7 +12452,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12460,7 +12460,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1094</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12468,7 +12468,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -12476,7 +12476,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -12484,7 +12484,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12492,7 +12492,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12500,7 +12500,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12508,7 +12508,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12516,7 +12516,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12524,7 +12524,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12532,7 +12532,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12540,7 +12540,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12548,7 +12548,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12556,7 +12556,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12564,7 +12564,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12572,7 +12572,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12580,7 +12580,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12588,7 +12588,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12596,7 +12596,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -12604,7 +12604,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12612,7 +12612,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12620,7 +12620,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12628,7 +12628,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -12636,7 +12636,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12660,7 +12660,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12668,7 +12668,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12676,7 +12676,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12684,7 +12684,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12692,7 +12692,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12700,7 +12700,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12708,7 +12708,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12716,7 +12716,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12724,7 +12724,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12732,7 +12732,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12740,7 +12740,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12772,7 +12772,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12820,7 +12820,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12828,7 +12828,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12844,7 +12844,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12852,7 +12852,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12860,7 +12860,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12868,7 +12868,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12916,7 +12916,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12924,7 +12924,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12932,7 +12932,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12940,7 +12940,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12948,7 +12948,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12956,7 +12956,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -12964,7 +12964,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12972,7 +12972,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12980,7 +12980,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12988,7 +12988,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12996,7 +12996,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -13004,7 +13004,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -13012,7 +13012,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13028,7 +13028,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -13036,7 +13036,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13044,7 +13044,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13052,7 +13052,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -13060,7 +13060,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -13068,7 +13068,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -13076,7 +13076,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13092,7 +13092,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -13100,7 +13100,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -13108,7 +13108,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -13116,7 +13116,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13132,7 +13132,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -13140,7 +13140,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -13148,7 +13148,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -13156,7 +13156,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
@@ -13164,7 +13164,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="360" x14ac:dyDescent="0.3">
@@ -13172,7 +13172,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13196,7 +13196,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -13204,7 +13204,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -13212,7 +13212,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13236,7 +13236,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -13244,7 +13244,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13252,7 +13252,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix display of disposing Huldra feat. Display r144f button on e203 if warrior boy held.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{070D18ED-53C0-497D-9751-5395ADA05AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{594437AD-4717-4D92-AEAA-434C4BB3B56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -8093,15 +8093,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content=' Fun Options ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e203 Daily Actions&lt;/Bold&gt;
- &lt;InlineUIContainer&gt; &lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r146a' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- &lt;InlineUIContainer&gt;&lt;Button Content='r144i' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Start of a new day! Select action button from the Daily Actions panel. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After all actions, events, food, and lodging are resolved, the day ends. This continues until the end of the 10th week, which ends the game.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;                &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sun3.gif' Height='220'  Width='440'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e211e Seeking an Audience with Lady Aeravir&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Lady Aeravir. Roll two die and consult the list below for results: 
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8131,6 +8122,16 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll die:
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll1' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e203 Daily Actions&lt;/Bold&gt;
+ &lt;InlineUIContainer&gt; &lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r146a' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ &lt;InlineUIContainer&gt;&lt;Button Content='r144f' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+ &lt;InlineUIContainer&gt;&lt;Button Content='r144i' FontFamily='Courier New' FontSize='12' Visibility='Hidden'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Start of a new day! Select action button from the Daily Actions panel. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After all actions, events, food, and lodging are resolved, the day ends. This continues until the end of the 10th week, which ends the game.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;                &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sun3.gif' Height='220'  Width='440'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8525,8 +8526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B415" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B416" sqref="B416"/>
+    <sheetView tabSelected="1" topLeftCell="B453" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B453" sqref="B453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11860,7 +11861,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12159,12 +12160,12 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="454" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A454" s="2" t="s">
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12460,7 +12461,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add Grammar corrections per glandmeade.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{594437AD-4717-4D92-AEAA-434C4BB3B56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{530C8519-5415-4E5D-8CD1-8A721AF95240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -8078,21 +8078,6 @@
                           &lt;InlineUIContainer&gt;&lt;Image Name='MountainPath' Source='../images/MountainPath.gif' Height='258' Width='280'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e001 The Adventure Begins&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Evil events have overtaken your Northlands Kingdom. Your father, the old king, is dead - assassinated by rivals to the throne.  These usurpers now hold the place with their mercenary royal guard. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You have escaped, and must collect 500 gold pieces to raise a force to smash them and retake your heritage. Furthermore, the usurpers have powerful friends overseas. If you can't return to take them out in ten weeks, their allies will arrive and you lose your kingdom forever. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-At dawn, you roll out of the merchant wagons into a ditch, dust off your clothes, loosen your swordbelt, and get ready to start the first day of your adventure &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The original game is brutally difficult to win. The &lt;Bold&gt;recommended&lt;/Bold&gt; fun game provides a random starting party, a random starting hex, food, and coins. Details can be viewed on the &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu where other game options can be selected. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you want different options, you must open the Options Dialog with &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu, and check the &lt;Bold&gt;AutoSetup&lt;/Bold&gt; checkbox. Then, select &lt;Bold&gt;File | New&lt;/Bold&gt; menu to start a new game with those options.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='Original Game' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-    or    
-&lt;InlineUIContainer&gt;&lt;Button Content=' Fun Options ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e211e Seeking an Audience with Lady Aeravir&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;As a daily action, you spend the day trying to gain admission to see the Lady Aeravir. Roll two die and consult the list below for results: 
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8132,6 +8117,21 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Start of a new day! Select action button from the Daily Actions panel. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;After all actions, events, food, and lodging are resolved, the day ends. This continues until the end of the 10th week, which ends the game.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;                &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sun3.gif' Height='220'  Width='440'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e001 The Adventure Begins&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Evil events have overtaken your Northlands Kingdom. Your father, the old king, is dead - assassinated by rivals to the throne.  These usurpers now hold the palace with their mercenary royal guard. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You have escaped, and must collect 500 gold pieces to raise a force to smash them and retake your heritage. Furthermore, the usurpers have powerful friends overseas. If you can't return to take them out in ten weeks, their allies will arrive and you lose your kingdom forever. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At dawn, you roll out of the merchant wagons into a ditch, dust off your clothes, loosen your swordbelt, and get ready to start the first day of your adventure &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The original game is brutally difficult to win. The &lt;Bold&gt;recommended&lt;/Bold&gt; fun game provides a random starting party, a random starting hex, food, and coins. Details can be viewed on the &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu where other game options can be selected. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you want different options, you must open the Options Dialog with &lt;Bold&gt;File | Options...&lt;/Bold&gt; menu, and check the &lt;Bold&gt;AutoSetup&lt;/Bold&gt; checkbox. Then, select &lt;Bold&gt;File | New&lt;/Bold&gt; menu to start a new game with those options.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Original Game' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+    or    
+&lt;InlineUIContainer&gt;&lt;Button Content=' Fun Options ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8526,8 +8526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B453" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B453" sqref="B453"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8581,7 +8581,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1176</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -11861,7 +11861,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12165,7 +12165,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12461,7 +12461,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix displaying PartyDisplay popup on DPI not equal to one. Fix display of BannderDialog not moving properly with DPI not equal to one.  Fix inital starting hex from 0801 to 0901.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{530C8519-5415-4E5D-8CD1-8A721AF95240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A2F0766-18DA-43B0-B109-787AD6BF246B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2481,22 +2481,6 @@
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll'  Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e001a Original Game Starting Location&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Italic&gt;Important Note:&lt;/Italic&gt; If you finish actions for a day on any hex north of the 
- &lt;InlineUIContainer&gt;&lt;Button Content='Tragoth River' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
-you may be found. See &lt;InlineUIContainer&gt;&lt;Button Content='e002' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-after normal events are concluded for the day, but before you take your evening meal.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll one die to see where you start: &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='0101' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 1 - Ogon
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='0701' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 2 
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='0801' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 - Ruins of Jakor's Keep
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='1301' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='1501' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 - Weshor
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='1801' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 6 </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e002 Mercenary Royal Guardsmen&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 As you prepare to rest for the night, you see mercenary royal guardsmen attempting to find you. Roll one die, subtract three, then add one if you are in Ogon 
@@ -8132,6 +8116,22 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Original Game' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
     or    
 &lt;InlineUIContainer&gt;&lt;Button Content=' Fun Options ' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e001a Original Game Starting Location&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Italic&gt;Important Note:&lt;/Italic&gt; If you finish actions for a day on any hex north of the 
+ &lt;InlineUIContainer&gt;&lt;Button Content='Tragoth River' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+you may be found. See &lt;InlineUIContainer&gt;&lt;Button Content='e002' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+after normal events are concluded for the day, but before you take your evening meal.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll one die to see where you start: &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='0101' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 1 - Ogon
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='0701' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 2 
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='0901' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 3 - Ruins of Jakor's Keep
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='1301' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 4 
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='1501' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 5 - Weshor
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Content='1801' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 6 </t>
   </si>
 </sst>
 </file>
@@ -8526,8 +8526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8549,7 +8549,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -8581,7 +8581,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8589,7 +8589,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>658</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8597,7 +8597,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8605,7 +8605,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8613,7 +8613,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8621,7 +8621,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8629,7 +8629,7 @@
         <v>258</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -8645,7 +8645,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -8653,7 +8653,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8661,7 +8661,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -8669,7 +8669,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8677,7 +8677,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8685,7 +8685,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8693,7 +8693,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -8701,7 +8701,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8709,7 +8709,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8717,7 +8717,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8725,7 +8725,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8733,7 +8733,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8741,7 +8741,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -8749,7 +8749,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -8757,7 +8757,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8765,7 +8765,7 @@
         <v>261</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -8773,7 +8773,7 @@
         <v>545</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -8781,7 +8781,7 @@
         <v>546</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -8789,7 +8789,7 @@
         <v>548</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -8797,7 +8797,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -8805,7 +8805,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8813,7 +8813,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -8821,7 +8821,7 @@
         <v>550</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -8829,7 +8829,7 @@
         <v>551</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8837,7 +8837,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8845,7 +8845,7 @@
         <v>557</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -8853,7 +8853,7 @@
         <v>558</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -8861,7 +8861,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8869,7 +8869,7 @@
         <v>262</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -8877,7 +8877,7 @@
         <v>263</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8885,7 +8885,7 @@
         <v>27</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -8893,7 +8893,7 @@
         <v>28</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -8901,7 +8901,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -8909,7 +8909,7 @@
         <v>30</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8917,7 +8917,7 @@
         <v>407</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8925,7 +8925,7 @@
         <v>502</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -8933,7 +8933,7 @@
         <v>31</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -8941,7 +8941,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -8949,7 +8949,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -8957,7 +8957,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8965,7 +8965,7 @@
         <v>408</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8973,7 +8973,7 @@
         <v>409</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -8981,7 +8981,7 @@
         <v>400</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -8989,7 +8989,7 @@
         <v>401</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -8997,7 +8997,7 @@
         <v>402</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9005,7 +9005,7 @@
         <v>264</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9013,7 +9013,7 @@
         <v>265</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9021,7 +9021,7 @@
         <v>404</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9029,7 +9029,7 @@
         <v>426</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9037,7 +9037,7 @@
         <v>35</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9045,7 +9045,7 @@
         <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9053,7 +9053,7 @@
         <v>405</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9061,7 +9061,7 @@
         <v>406</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9069,7 +9069,7 @@
         <v>37</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -9085,7 +9085,7 @@
         <v>43</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9093,7 +9093,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9101,7 +9101,7 @@
         <v>503</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9109,7 +9109,7 @@
         <v>504</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9117,7 +9117,7 @@
         <v>39</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -9125,7 +9125,7 @@
         <v>40</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9133,7 +9133,7 @@
         <v>41</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9141,7 +9141,7 @@
         <v>45</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9149,7 +9149,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9157,7 +9157,7 @@
         <v>46</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9165,7 +9165,7 @@
         <v>47</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9173,7 +9173,7 @@
         <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -9181,7 +9181,7 @@
         <v>49</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9189,7 +9189,7 @@
         <v>50</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9197,7 +9197,7 @@
         <v>51</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9205,7 +9205,7 @@
         <v>52</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9213,7 +9213,7 @@
         <v>53</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -9221,7 +9221,7 @@
         <v>54</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9229,7 +9229,7 @@
         <v>55</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9237,7 +9237,7 @@
         <v>56</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9245,7 +9245,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9253,7 +9253,7 @@
         <v>58</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9261,7 +9261,7 @@
         <v>523</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9269,7 +9269,7 @@
         <v>524</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9277,7 +9277,7 @@
         <v>527</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9285,7 +9285,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9293,7 +9293,7 @@
         <v>556</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9301,7 +9301,7 @@
         <v>60</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9309,7 +9309,7 @@
         <v>522</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9317,7 +9317,7 @@
         <v>61</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9325,7 +9325,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9333,7 +9333,7 @@
         <v>341</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9341,7 +9341,7 @@
         <v>63</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9349,7 +9349,7 @@
         <v>64</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9357,7 +9357,7 @@
         <v>65</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -9365,7 +9365,7 @@
         <v>66</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9373,7 +9373,7 @@
         <v>329</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9381,7 +9381,7 @@
         <v>67</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9389,7 +9389,7 @@
         <v>386</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9397,7 +9397,7 @@
         <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9405,7 +9405,7 @@
         <v>342</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9413,7 +9413,7 @@
         <v>387</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9421,7 +9421,7 @@
         <v>69</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9429,7 +9429,7 @@
         <v>390</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9437,7 +9437,7 @@
         <v>391</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9445,7 +9445,7 @@
         <v>70</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -9453,7 +9453,7 @@
         <v>343</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9461,7 +9461,7 @@
         <v>259</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9469,7 +9469,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9477,7 +9477,7 @@
         <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9485,7 +9485,7 @@
         <v>73</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9501,7 +9501,7 @@
         <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9517,7 +9517,7 @@
         <v>324</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9525,7 +9525,7 @@
         <v>621</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -9533,7 +9533,7 @@
         <v>76</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9541,7 +9541,7 @@
         <v>77</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9565,7 +9565,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9573,7 +9573,7 @@
         <v>349</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9581,7 +9581,7 @@
         <v>350</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9589,7 +9589,7 @@
         <v>79</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9597,7 +9597,7 @@
         <v>346</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9605,7 +9605,7 @@
         <v>347</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9613,7 +9613,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9621,7 +9621,7 @@
         <v>81</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9629,7 +9629,7 @@
         <v>568</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9637,7 +9637,7 @@
         <v>569</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9645,7 +9645,7 @@
         <v>570</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9653,7 +9653,7 @@
         <v>571</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9661,7 +9661,7 @@
         <v>572</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9669,7 +9669,7 @@
         <v>573</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9677,7 +9677,7 @@
         <v>574</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9685,7 +9685,7 @@
         <v>575</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9693,7 +9693,7 @@
         <v>576</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9701,7 +9701,7 @@
         <v>577</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9709,7 +9709,7 @@
         <v>82</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9717,7 +9717,7 @@
         <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -9725,7 +9725,7 @@
         <v>601</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -9733,7 +9733,7 @@
         <v>84</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9741,7 +9741,7 @@
         <v>85</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9749,7 +9749,7 @@
         <v>425</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9757,7 +9757,7 @@
         <v>634</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9765,7 +9765,7 @@
         <v>86</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9773,7 +9773,7 @@
         <v>87</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9781,7 +9781,7 @@
         <v>333</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9789,7 +9789,7 @@
         <v>370</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
@@ -9797,7 +9797,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9805,7 +9805,7 @@
         <v>334</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9813,7 +9813,7 @@
         <v>335</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9821,7 +9821,7 @@
         <v>336</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9829,7 +9829,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9837,7 +9837,7 @@
         <v>337</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9845,7 +9845,7 @@
         <v>339</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9853,7 +9853,7 @@
         <v>340</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -9861,7 +9861,7 @@
         <v>509</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9869,7 +9869,7 @@
         <v>89</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9877,7 +9877,7 @@
         <v>375</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9885,7 +9885,7 @@
         <v>376</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9893,7 +9893,7 @@
         <v>379</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -9901,7 +9901,7 @@
         <v>90</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -9909,7 +9909,7 @@
         <v>535</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9917,7 +9917,7 @@
         <v>536</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -9925,7 +9925,7 @@
         <v>91</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9933,7 +9933,7 @@
         <v>380</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9941,7 +9941,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9949,7 +9949,7 @@
         <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
@@ -9973,7 +9973,7 @@
         <v>96</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -9981,7 +9981,7 @@
         <v>540</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -9989,7 +9989,7 @@
         <v>541</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -9997,7 +9997,7 @@
         <v>542</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10005,7 +10005,7 @@
         <v>543</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10013,7 +10013,7 @@
         <v>547</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10029,7 +10029,7 @@
         <v>97</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10037,7 +10037,7 @@
         <v>98</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10045,7 +10045,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10053,7 +10053,7 @@
         <v>101</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10061,7 +10061,7 @@
         <v>100</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10069,7 +10069,7 @@
         <v>102</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10077,7 +10077,7 @@
         <v>103</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10085,7 +10085,7 @@
         <v>104</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10093,7 +10093,7 @@
         <v>105</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10101,7 +10101,7 @@
         <v>500</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10109,7 +10109,7 @@
         <v>501</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10117,7 +10117,7 @@
         <v>106</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10125,7 +10125,7 @@
         <v>107</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10133,7 +10133,7 @@
         <v>165</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -10141,7 +10141,7 @@
         <v>537</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -10149,7 +10149,7 @@
         <v>108</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
@@ -10157,7 +10157,7 @@
         <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -10165,7 +10165,7 @@
         <v>110</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10173,7 +10173,7 @@
         <v>166</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10181,7 +10181,7 @@
         <v>167</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -10189,7 +10189,7 @@
         <v>168</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10197,7 +10197,7 @@
         <v>552</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10213,7 +10213,7 @@
         <v>111</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10221,7 +10221,7 @@
         <v>506</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -10229,7 +10229,7 @@
         <v>507</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -10245,7 +10245,7 @@
         <v>512</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10253,7 +10253,7 @@
         <v>112</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10261,7 +10261,7 @@
         <v>169</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10269,7 +10269,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10277,7 +10277,7 @@
         <v>171</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -10285,7 +10285,7 @@
         <v>113</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10293,7 +10293,7 @@
         <v>114</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10301,7 +10301,7 @@
         <v>266</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10309,7 +10309,7 @@
         <v>559</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10317,7 +10317,7 @@
         <v>115</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10325,7 +10325,7 @@
         <v>518</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -10333,7 +10333,7 @@
         <v>116</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10341,7 +10341,7 @@
         <v>516</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10349,7 +10349,7 @@
         <v>117</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10357,7 +10357,7 @@
         <v>519</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10365,7 +10365,7 @@
         <v>520</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10373,7 +10373,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10381,7 +10381,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -10389,7 +10389,7 @@
         <v>562</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10397,7 +10397,7 @@
         <v>563</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10405,7 +10405,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10413,7 +10413,7 @@
         <v>555</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10421,7 +10421,7 @@
         <v>554</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10429,7 +10429,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10437,7 +10437,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10445,7 +10445,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10453,7 +10453,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -10461,7 +10461,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10469,7 +10469,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10477,7 +10477,7 @@
         <v>517</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10485,7 +10485,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10493,7 +10493,7 @@
         <v>560</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10501,7 +10501,7 @@
         <v>561</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10509,7 +10509,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10517,7 +10517,7 @@
         <v>604</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10525,7 +10525,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10533,7 +10533,7 @@
         <v>578</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10541,7 +10541,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -10549,7 +10549,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10557,7 +10557,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10565,7 +10565,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10573,7 +10573,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10581,7 +10581,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -10589,7 +10589,7 @@
         <v>565</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10597,7 +10597,7 @@
         <v>566</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10605,7 +10605,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10613,7 +10613,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10621,7 +10621,7 @@
         <v>564</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -10629,7 +10629,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10637,7 +10637,7 @@
         <v>579</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10645,7 +10645,7 @@
         <v>580</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10653,7 +10653,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -10661,7 +10661,7 @@
         <v>581</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10669,7 +10669,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10677,7 +10677,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10685,7 +10685,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10693,7 +10693,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -10709,7 +10709,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10717,7 +10717,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -10733,7 +10733,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10741,7 +10741,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10749,7 +10749,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10765,7 +10765,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10773,7 +10773,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10781,7 +10781,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10789,7 +10789,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10797,7 +10797,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10805,7 +10805,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -10813,7 +10813,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10821,7 +10821,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10829,7 +10829,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10837,7 +10837,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10845,7 +10845,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10853,7 +10853,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -10861,7 +10861,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10869,7 +10869,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10877,7 +10877,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -10885,7 +10885,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10893,7 +10893,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10901,7 +10901,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -10909,7 +10909,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10917,7 +10917,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10925,7 +10925,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10933,7 +10933,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10941,7 +10941,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10949,7 +10949,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -10957,7 +10957,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -10965,7 +10965,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -10973,7 +10973,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -10989,7 +10989,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -10997,7 +10997,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -11005,7 +11005,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11021,7 +11021,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11029,7 +11029,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -11037,7 +11037,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11045,7 +11045,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11053,7 +11053,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11061,7 +11061,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11069,7 +11069,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11077,7 +11077,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11085,7 +11085,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11093,7 +11093,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11101,7 +11101,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="360" x14ac:dyDescent="0.3">
@@ -11109,7 +11109,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -11125,7 +11125,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11133,7 +11133,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -11141,7 +11141,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11149,7 +11149,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11157,7 +11157,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11165,7 +11165,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
@@ -11173,7 +11173,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -11189,7 +11189,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11197,7 +11197,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -11205,7 +11205,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -11213,7 +11213,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -11221,7 +11221,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11229,7 +11229,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11237,7 +11237,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -11245,7 +11245,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11253,7 +11253,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11261,7 +11261,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11269,7 +11269,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11277,7 +11277,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11285,7 +11285,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11301,7 +11301,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11309,7 +11309,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11317,7 +11317,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -11333,7 +11333,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11341,7 +11341,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -11349,7 +11349,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11365,7 +11365,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -11373,7 +11373,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11381,7 +11381,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11389,7 +11389,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -11397,7 +11397,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11405,7 +11405,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -11413,7 +11413,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11421,7 +11421,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -11429,7 +11429,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -11445,7 +11445,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11453,7 +11453,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -11461,7 +11461,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11469,7 +11469,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11477,7 +11477,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11485,7 +11485,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11493,7 +11493,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11501,7 +11501,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11509,7 +11509,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -11517,7 +11517,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -11525,7 +11525,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11533,7 +11533,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11541,7 +11541,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -11549,7 +11549,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11557,7 +11557,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11565,7 +11565,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11573,7 +11573,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11581,7 +11581,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11589,7 +11589,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11597,7 +11597,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11605,7 +11605,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11613,7 +11613,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -11661,7 +11661,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11669,7 +11669,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11677,7 +11677,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11685,7 +11685,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11693,7 +11693,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -11701,7 +11701,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11709,7 +11709,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11717,7 +11717,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -11789,7 +11789,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -11797,7 +11797,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11805,7 +11805,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11813,7 +11813,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11821,7 +11821,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11829,7 +11829,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11837,7 +11837,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11845,7 +11845,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11853,7 +11853,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -11861,7 +11861,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -11869,7 +11869,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11877,7 +11877,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11885,7 +11885,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11893,7 +11893,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11901,7 +11901,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11909,7 +11909,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11917,7 +11917,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11925,7 +11925,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -11933,7 +11933,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -11941,7 +11941,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -11949,7 +11949,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="288" x14ac:dyDescent="0.3">
@@ -11957,7 +11957,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11965,7 +11965,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11973,7 +11973,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -11981,7 +11981,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -11989,7 +11989,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -11997,7 +11997,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12005,7 +12005,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12013,7 +12013,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12021,7 +12021,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12029,7 +12029,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12037,7 +12037,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12045,7 +12045,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12053,7 +12053,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12061,7 +12061,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12069,7 +12069,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12077,7 +12077,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12085,7 +12085,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12093,7 +12093,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12101,7 +12101,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12109,7 +12109,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -12117,7 +12117,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12125,7 +12125,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12133,7 +12133,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12141,7 +12141,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12149,7 +12149,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -12157,7 +12157,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12165,7 +12165,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12173,7 +12173,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12181,7 +12181,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12189,7 +12189,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12205,7 +12205,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -12253,7 +12253,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12261,7 +12261,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12269,7 +12269,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12277,7 +12277,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12285,7 +12285,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12293,7 +12293,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12301,7 +12301,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12309,7 +12309,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12317,7 +12317,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12325,7 +12325,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -12333,7 +12333,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12341,7 +12341,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -12349,7 +12349,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12357,7 +12357,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12365,7 +12365,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12373,7 +12373,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12381,7 +12381,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12389,7 +12389,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12397,7 +12397,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12405,7 +12405,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12413,7 +12413,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -12421,7 +12421,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -12429,7 +12429,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12437,7 +12437,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12445,7 +12445,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12453,7 +12453,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12461,7 +12461,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12469,7 +12469,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -12477,7 +12477,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -12485,7 +12485,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12493,7 +12493,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12501,7 +12501,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12509,7 +12509,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12517,7 +12517,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12525,7 +12525,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12533,7 +12533,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12541,7 +12541,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12549,7 +12549,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -12557,7 +12557,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12565,7 +12565,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12573,7 +12573,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -12581,7 +12581,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12589,7 +12589,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12597,7 +12597,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -12605,7 +12605,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12613,7 +12613,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12621,7 +12621,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12629,7 +12629,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -12637,7 +12637,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12661,7 +12661,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12669,7 +12669,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12677,7 +12677,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12685,7 +12685,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12693,7 +12693,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12701,7 +12701,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12709,7 +12709,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12717,7 +12717,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12725,7 +12725,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12733,7 +12733,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -12741,7 +12741,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12773,7 +12773,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12821,7 +12821,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12829,7 +12829,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -12845,7 +12845,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12853,7 +12853,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12861,7 +12861,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12869,7 +12869,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12917,7 +12917,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12925,7 +12925,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12933,7 +12933,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12941,7 +12941,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
@@ -12949,7 +12949,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12957,7 +12957,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -12965,7 +12965,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -12973,7 +12973,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -12981,7 +12981,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -12989,7 +12989,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -12997,7 +12997,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -13005,7 +13005,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -13013,7 +13013,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13029,7 +13029,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -13037,7 +13037,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13045,7 +13045,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13053,7 +13053,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -13061,7 +13061,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -13069,7 +13069,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -13077,7 +13077,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13093,7 +13093,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -13101,7 +13101,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -13109,7 +13109,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -13117,7 +13117,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13133,7 +13133,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -13141,7 +13141,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -13149,7 +13149,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -13157,7 +13157,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
@@ -13165,7 +13165,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="360" x14ac:dyDescent="0.3">
@@ -13173,7 +13173,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13197,7 +13197,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -13205,7 +13205,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -13213,7 +13213,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -13237,7 +13237,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -13245,7 +13245,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -13253,7 +13253,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event e036 allows golem to strike first. Resurrection of Prince when he is alone and dies in combat. Fix e212i showing wrong content for t226.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAB0435A-E5D9-4BB1-8E91-88CDD618F761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDD5683E-6B43-4037-B0B5-838AE65419E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="16520" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -7326,18 +7326,6 @@
                    &lt;InlineUIContainer&gt;&lt;Image Source='../images/Temple.gif' Name='Temple' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e212i Fall in Love with Priestess&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You find true love
- &lt;InlineUIContainer&gt;&lt;Button Content='r228' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You immediately escape
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- with her and can never return to this hex. She has a combat skill 2 and endurance 4. Her wealth is 100 wealth code
- &lt;InlineUIContainer&gt;&lt;Button Content='r226' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- which she has stolen from the temple treasure! Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                  &lt;InlineUIContainer&gt;&lt;Image Source='../images/PriestDaughter.gif' Name='LordsDaughterLove' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e212j  High Priest Request Audience&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;High Priestess requests an audience
  &lt;InlineUIContainer&gt;&lt;Button Content='e155' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
@@ -8134,6 +8122,18 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Dismiss' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; a random magic user from party to add one to die roll.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll two die and consult list for results:  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e212i Fall in Love with Priestess&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You find true love
+ &lt;InlineUIContainer&gt;&lt;Button Content='r228' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You immediately escape
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with her and can never return to this hex. She has a combat skill 2 and endurance 4. Her wealth is 100 wealth code
+ &lt;InlineUIContainer&gt;&lt;Button Content='t226' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ which she has stolen from the temple treasure! Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                  &lt;InlineUIContainer&gt;&lt;Image Source='../images/PriestDaughter.gif' Name='LordsDaughterLove' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8528,8 +8528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B488" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B488" sqref="B488"/>
+    <sheetView tabSelected="1" topLeftCell="B502" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B503" sqref="B503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8551,7 +8551,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8583,7 +8583,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8591,7 +8591,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9943,7 +9943,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1102</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12623,7 +12623,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12631,7 +12631,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12639,7 +12639,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12663,7 +12663,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12671,7 +12671,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12679,7 +12679,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12687,7 +12687,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12711,7 +12711,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12775,7 +12775,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12959,7 +12959,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12999,7 +12999,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13055,7 +13055,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13063,7 +13063,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13095,7 +13095,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13103,7 +13103,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13111,7 +13111,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13119,7 +13119,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13135,7 +13135,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13143,7 +13143,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13151,7 +13151,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13159,7 +13159,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13167,7 +13167,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13175,7 +13175,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13199,7 +13199,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13207,7 +13207,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13215,7 +13215,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13239,7 +13239,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13247,7 +13247,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13255,7 +13255,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix spelling error with Drogatt. Fix only reporting GameFeat if number is above zero.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDD5683E-6B43-4037-B0B5-838AE65419E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C09F985-A9B8-4134-82C0-440EFEBCB93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="16520" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -5890,29 +5890,6 @@
                            &lt;InlineUIContainer&gt;&lt;Image Source='../images/Caravan.gif' Name='EncounterEnd' Height='150'  Width='300'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e130 Meet the High Lord&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You meet a high and powerful lord of the land. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The Lord has one or more bodyguards. Each has a combat skill 6 and endurance 6.  Roll two dice and add one for the number of guards:
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll one die for identity:  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;
- 1 - Baron of Huldra Castle&lt;LineBreak/&gt;
- 2 - Count Drogatt of Drogat Castle&lt;LineBreak/&gt;
- 3 - Lady Aeravir of Aeravir Castle&lt;LineBreak/&gt;
- 4 - High Priest of a Temple&lt;LineBreak/&gt;
- 5,6 - Town Mayor
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-To advance to next screen, select one of the buttons labeled: Talk, Evade, Fight:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12'  Content='Talk ' Name='e130a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Evade' Name='e130b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e130c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
- &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e130a Talk to High Lord&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
  &lt;InlineUIContainer&gt;&lt;Button Content='e327' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Pass&lt;LineBreak/&gt;
@@ -8134,6 +8111,29 @@
  which she has stolen from the temple treasure! Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/PriestDaughter.gif' Name='LordsDaughterLove' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e130 Meet the High Lord&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You meet a high and powerful lord of the land. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The Lord has one or more bodyguards. Each has a combat skill 6 and endurance 6.  Roll two dice and add one for the number of guards:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DiceRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll one die for identity:  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;
+ 1 - Baron of Huldra Castle&lt;LineBreak/&gt;
+ 2 - Count Drogat of Drogat Castle&lt;LineBreak/&gt;
+ 3 - Lady Aeravir of Aeravir Castle&lt;LineBreak/&gt;
+ 4 - High Priest of a Temple&lt;LineBreak/&gt;
+ 5,6 - Town Mayor
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+To advance to next screen, select one of the buttons labeled: Talk, Evade, Fight:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12'  Content='Talk ' Name='e130a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130a'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Evade' Name='e130b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e130c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
+ &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8528,8 +8528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B502" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B503" sqref="B503"/>
+    <sheetView tabSelected="1" topLeftCell="B333" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B334" sqref="B334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8551,7 +8551,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8583,7 +8583,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8591,7 +8591,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9943,7 +9943,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11207,7 +11207,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>962</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11239,7 +11239,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11319,7 +11319,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11503,7 +11503,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11511,7 +11511,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11519,7 +11519,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11527,7 +11527,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11535,7 +11535,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11607,7 +11607,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11615,7 +11615,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11663,7 +11663,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="285.3" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12079,7 +12079,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12087,7 +12087,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12095,7 +12095,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12103,7 +12103,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12111,7 +12111,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -12119,7 +12119,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12127,7 +12127,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12519,7 +12519,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12527,7 +12527,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12623,7 +12623,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12631,7 +12631,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12639,7 +12639,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12663,7 +12663,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12671,7 +12671,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12679,7 +12679,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12687,7 +12687,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12711,7 +12711,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12775,7 +12775,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12959,7 +12959,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12999,7 +12999,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13055,7 +13055,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13063,7 +13063,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13095,7 +13095,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13103,7 +13103,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13111,7 +13111,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13119,7 +13119,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13135,7 +13135,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13143,7 +13143,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13151,7 +13151,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13159,7 +13159,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13167,7 +13167,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13175,7 +13175,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13199,7 +13199,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13207,7 +13207,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13215,7 +13215,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13239,7 +13239,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13247,7 +13247,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13255,7 +13255,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
If defeat Hill Tribe, set rescue heir game feat to true.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C09F985-A9B8-4134-82C0-440EFEBCB93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BEE148F-CA52-4AB8-87D9-4C16401E1B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -6194,18 +6194,6 @@
                    &lt;InlineUIContainer&gt;&lt;Image Source='../images/CrossedSwords.gif' Name='HeirRescue' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e144c Escape with True Heir to Huldra Castle&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After either using the an item or killing the guards, you can escape
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- from the hill tribe in
- &lt;InlineUIContainer&gt;&lt;Button Content='1611' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. You escape
- with the true heir who has combat skill 5 and endurance 7.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Next, take the heir to the Huldra castle.  See  &lt;InlineUIContainer&gt;&lt;Button Content='e144d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you get there. Click the image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Source='../images/WarriorBoy.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e144d Travel with Heir to Huldra Castle&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You travel with the heir. If you reach Huldra Castle, your party and the heir have two options.&lt;LineBreak/&gt;
@@ -8134,6 +8122,18 @@
  &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130b'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
  &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e130c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
  &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e130c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e144c Escape with True Heir to Huldra Castle&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After either using an item or killing the guards, you can escape
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ from the hill tribe in
+ &lt;InlineUIContainer&gt;&lt;Button Content='1611' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. You escape
+ with the true heir who has combat skill 5 and endurance 7.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Next, take the heir to the Huldra castle.  See  &lt;InlineUIContainer&gt;&lt;Button Content='e144d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you get there. Click the image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Source='../images/WarriorBoy.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8528,8 +8528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B333" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B334" sqref="B334"/>
+    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B365" sqref="B365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8551,7 +8551,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8583,7 +8583,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8591,7 +8591,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9943,7 +9943,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11207,7 +11207,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>988</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11503,7 +11503,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11511,7 +11511,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11519,7 +11519,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11527,7 +11527,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11535,7 +11535,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11607,7 +11607,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11615,7 +11615,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11663,7 +11663,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="285.3" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12079,7 +12079,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12087,7 +12087,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12095,7 +12095,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12103,7 +12103,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12111,7 +12111,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -12119,7 +12119,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12127,7 +12127,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12519,7 +12519,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12527,7 +12527,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12623,7 +12623,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12631,7 +12631,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12639,7 +12639,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12663,7 +12663,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12671,7 +12671,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12679,7 +12679,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12687,7 +12687,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12711,7 +12711,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12775,7 +12775,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12959,7 +12959,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12999,7 +12999,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13055,7 +13055,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13063,7 +13063,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13095,7 +13095,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13103,7 +13103,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13111,7 +13111,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13119,7 +13119,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13135,7 +13135,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13143,7 +13143,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13151,7 +13151,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13159,7 +13159,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13167,7 +13167,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13175,7 +13175,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13199,7 +13199,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13207,7 +13207,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13215,7 +13215,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13239,7 +13239,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13247,7 +13247,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13255,7 +13255,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
When loading game file, set g.NewHex to current territory. Support the UpdateGameOptions when in Setup game phase.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BEE148F-CA52-4AB8-87D9-4C16401E1B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7E360AE-3BA4-4116-90AC-6BCD248E2FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -5327,21 +5327,6 @@
                                   &lt;InlineUIContainer&gt;&lt;Image Name='E100EncounterFight' Source='../images/Griffon.gif' Height='250' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e101a Talk to Harpy&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r342' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Inquiry&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r329' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Pass&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r340' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 aand 4 - Looter&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r308' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Surprised&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r310' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Surprised
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll die:
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll1' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll2' Height='21'  Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;
-                             &lt;InlineUIContainer&gt;&lt;Image Name='E101EncounterTalk' Source='../images/Harpy.gif' Height='300'  Width='265' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e101b Evade Harpy&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die: 
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
@@ -8134,6 +8119,21 @@
 Next, take the heir to the Huldra castle.  See  &lt;InlineUIContainer&gt;&lt;Button Content='e144d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; when you get there. Click the image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Source='../images/WarriorBoy.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e101a Talk to Harpy&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r342' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Inquiry&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r329' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Pass&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r340' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 and 4 - Looter&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r308' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Surprised&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r310' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Surprised
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll die:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll1' Height='21'  Width='21'  Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll2' Height='21'  Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;
+                             &lt;InlineUIContainer&gt;&lt;Image Name='E101EncounterTalk' Source='../images/Harpy.gif' Height='300'  Width='265' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8528,8 +8528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B365" sqref="B365"/>
+    <sheetView tabSelected="1" topLeftCell="B278" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8551,7 +8551,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8583,7 +8583,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8591,7 +8591,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9943,7 +9943,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10375,7 +10375,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10463,7 +10463,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10471,7 +10471,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10767,7 +10767,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>911</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10775,7 +10775,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10783,7 +10783,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10791,7 +10791,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10799,7 +10799,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10815,7 +10815,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10823,7 +10823,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10831,7 +10831,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10839,7 +10839,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10847,7 +10847,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10863,7 +10863,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10879,7 +10879,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10887,7 +10887,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10895,7 +10895,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10911,7 +10911,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10919,7 +10919,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10927,7 +10927,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10935,7 +10935,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10951,7 +10951,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10959,7 +10959,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10967,7 +10967,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10975,7 +10975,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10999,7 +10999,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11007,7 +11007,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11023,7 +11023,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11031,7 +11031,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11039,7 +11039,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11047,7 +11047,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11055,7 +11055,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11063,7 +11063,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11071,7 +11071,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11079,7 +11079,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11095,7 +11095,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11127,7 +11127,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11135,7 +11135,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11143,7 +11143,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11151,7 +11151,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11159,7 +11159,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11167,7 +11167,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="370.9" x14ac:dyDescent="0.25">
@@ -11175,7 +11175,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11191,7 +11191,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11199,7 +11199,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="299.55" x14ac:dyDescent="0.25">
@@ -11207,7 +11207,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11215,7 +11215,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11223,7 +11223,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11231,7 +11231,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11239,7 +11239,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11247,7 +11247,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11255,7 +11255,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11263,7 +11263,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11271,7 +11271,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11279,7 +11279,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11287,7 +11287,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11311,7 +11311,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11319,7 +11319,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11335,7 +11335,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11343,7 +11343,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11351,7 +11351,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11367,7 +11367,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11375,7 +11375,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11383,7 +11383,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11391,7 +11391,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11407,7 +11407,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11423,7 +11423,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11431,7 +11431,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11447,7 +11447,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11455,7 +11455,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11463,7 +11463,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11471,7 +11471,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11479,7 +11479,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11487,7 +11487,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11503,7 +11503,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11511,7 +11511,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11519,7 +11519,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11527,7 +11527,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11535,7 +11535,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11543,7 +11543,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11551,7 +11551,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11567,7 +11567,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11575,7 +11575,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11583,7 +11583,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11591,7 +11591,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11599,7 +11599,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11607,7 +11607,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11615,7 +11615,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11663,7 +11663,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11671,7 +11671,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11679,7 +11679,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11687,7 +11687,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11695,7 +11695,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11703,7 +11703,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11719,7 +11719,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11799,7 +11799,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11815,7 +11815,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11823,7 +11823,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11831,7 +11831,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11839,7 +11839,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11847,7 +11847,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11855,7 +11855,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11863,7 +11863,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11871,7 +11871,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11879,7 +11879,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11911,7 +11911,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11919,7 +11919,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11935,7 +11935,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11943,7 +11943,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11951,7 +11951,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="285.3" x14ac:dyDescent="0.25">
@@ -11959,7 +11959,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11967,7 +11967,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11983,7 +11983,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11999,7 +11999,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12007,7 +12007,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12023,7 +12023,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12031,7 +12031,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12039,7 +12039,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12047,7 +12047,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12055,7 +12055,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12063,7 +12063,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12071,7 +12071,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12079,7 +12079,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12087,7 +12087,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12095,7 +12095,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12103,7 +12103,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12111,7 +12111,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -12119,7 +12119,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12127,7 +12127,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12135,7 +12135,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12143,7 +12143,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12151,7 +12151,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12159,7 +12159,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12167,7 +12167,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12175,7 +12175,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12191,7 +12191,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12207,7 +12207,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -12255,7 +12255,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12263,7 +12263,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12271,7 +12271,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12279,7 +12279,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12287,7 +12287,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12295,7 +12295,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12303,7 +12303,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12311,7 +12311,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12327,7 +12327,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12335,7 +12335,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12343,7 +12343,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12351,7 +12351,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12359,7 +12359,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12367,7 +12367,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12375,7 +12375,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12383,7 +12383,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12391,7 +12391,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12399,7 +12399,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12407,7 +12407,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12415,7 +12415,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12423,7 +12423,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12431,7 +12431,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12439,7 +12439,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -12447,7 +12447,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12455,7 +12455,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12463,7 +12463,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12479,7 +12479,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12487,7 +12487,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12495,7 +12495,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12503,7 +12503,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12511,7 +12511,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12519,7 +12519,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12527,7 +12527,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12535,7 +12535,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12543,7 +12543,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12559,7 +12559,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12567,7 +12567,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12575,7 +12575,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12583,7 +12583,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12591,7 +12591,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12599,7 +12599,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12607,7 +12607,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12615,7 +12615,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12623,7 +12623,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12631,7 +12631,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12639,7 +12639,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12663,7 +12663,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12671,7 +12671,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12679,7 +12679,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12687,7 +12687,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12695,7 +12695,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12703,7 +12703,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12711,7 +12711,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12719,7 +12719,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12727,7 +12727,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12735,7 +12735,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12775,7 +12775,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12823,7 +12823,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12831,7 +12831,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12847,7 +12847,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12855,7 +12855,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12863,7 +12863,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12871,7 +12871,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12919,7 +12919,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12943,7 +12943,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12951,7 +12951,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12959,7 +12959,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12967,7 +12967,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12975,7 +12975,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12983,7 +12983,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12991,7 +12991,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12999,7 +12999,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13007,7 +13007,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13015,7 +13015,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13039,7 +13039,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13047,7 +13047,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13055,7 +13055,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13063,7 +13063,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13071,7 +13071,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13079,7 +13079,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13095,7 +13095,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13103,7 +13103,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13111,7 +13111,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13119,7 +13119,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13135,7 +13135,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13143,7 +13143,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13151,7 +13151,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13159,7 +13159,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13167,7 +13167,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13175,7 +13175,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13199,7 +13199,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13207,7 +13207,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13215,7 +13215,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13239,7 +13239,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13247,7 +13247,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13255,7 +13255,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shrink Stone.gif image. Fix issue with e059 dwarf mines showing up twice.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7E360AE-3BA4-4116-90AC-6BCD248E2FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFAB05BA-0F6A-4979-B1F9-71937C92DAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -3784,19 +3784,6 @@
                                                 &lt;InlineUIContainer&gt;&lt;Image  Name='E037EncounterRoll' Source='../images/Chest2.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e038 Cache under Stone&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;By chance, you overturn a stone slab, As you jump back, it crashes to the ground. You see that it uncovers an old cache of rotting food  and other items. Roll one die:
- &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- 1 - &lt;InlineUIContainer&gt;&lt;Button Content='e180' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 2 - &lt;InlineUIContainer&gt;&lt;Button Content='e181' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 3 - &lt;InlineUIContainer&gt;&lt;Button Content='e182' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 4 - &lt;InlineUIContainer&gt;&lt;Button Content='e185' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 5 - &lt;InlineUIContainer&gt;&lt;Button Content='e187' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
- 6 - &lt;InlineUIContainer&gt;&lt;Button Content='e190' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='E038EncounterRoll' Source='../images/Stone.gif' Height='320'  Width='600'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e039 Small Treasure Chest&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You find a locked chest. You know the lock may be booby trapped.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='TreasureChest'  Source='../images/Chest.gif' Height='75'  Width='75'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; Click the chest to open.
@@ -8134,6 +8121,20 @@
  &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll2' Height='21'  Width='21' Visibility='Hidden'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;
                              &lt;InlineUIContainer&gt;&lt;Image Name='E101EncounterTalk' Source='../images/Harpy.gif' Height='300'  Width='265' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e038 Cache under Stone&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;By chance, you overturn a stone slab, As you jump back, it crashes to the ground. You see that it uncovers an old cache of rotting food  and other items. Roll one die:
+ &lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21' Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ 1 - &lt;InlineUIContainer&gt;&lt;Button Content='e180' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 2 - &lt;InlineUIContainer&gt;&lt;Button Content='e181' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 3 - &lt;InlineUIContainer&gt;&lt;Button Content='e182' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 4 - &lt;InlineUIContainer&gt;&lt;Button Content='e185' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 5 - &lt;InlineUIContainer&gt;&lt;Button Content='e187' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+ 6 - &lt;InlineUIContainer&gt;&lt;Button Content='e190' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;
+        &lt;InlineUIContainer&gt;&lt;Image Name='E038EncounterRoll' Source='../images/Stone.gif' Height='280'  Width='525'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -8528,8 +8529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B278" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B278" sqref="B278"/>
+    <sheetView tabSelected="1" topLeftCell="B116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8551,7 +8552,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8583,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8591,7 +8592,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9466,12 +9467,12 @@
         <v>764</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>765</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9479,7 +9480,7 @@
         <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9487,7 +9488,7 @@
         <v>73</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9503,7 +9504,7 @@
         <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9519,7 +9520,7 @@
         <v>324</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9527,7 +9528,7 @@
         <v>621</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -9535,7 +9536,7 @@
         <v>76</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9543,7 +9544,7 @@
         <v>77</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -9567,7 +9568,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9575,7 +9576,7 @@
         <v>349</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9583,7 +9584,7 @@
         <v>350</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9591,7 +9592,7 @@
         <v>79</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9599,7 +9600,7 @@
         <v>346</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9607,7 +9608,7 @@
         <v>347</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9615,7 +9616,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9623,7 +9624,7 @@
         <v>81</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9631,7 +9632,7 @@
         <v>568</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9639,7 +9640,7 @@
         <v>569</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9647,7 +9648,7 @@
         <v>570</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9655,7 +9656,7 @@
         <v>571</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9663,7 +9664,7 @@
         <v>572</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9671,7 +9672,7 @@
         <v>573</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9679,7 +9680,7 @@
         <v>574</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9687,7 +9688,7 @@
         <v>575</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9695,7 +9696,7 @@
         <v>576</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9703,7 +9704,7 @@
         <v>577</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9711,7 +9712,7 @@
         <v>82</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9719,7 +9720,7 @@
         <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9727,7 +9728,7 @@
         <v>601</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -9735,7 +9736,7 @@
         <v>84</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9743,7 +9744,7 @@
         <v>85</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9751,7 +9752,7 @@
         <v>425</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9759,7 +9760,7 @@
         <v>634</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9767,7 +9768,7 @@
         <v>86</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9775,7 +9776,7 @@
         <v>87</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9783,7 +9784,7 @@
         <v>333</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9791,7 +9792,7 @@
         <v>370</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="328.1" x14ac:dyDescent="0.25">
@@ -9799,7 +9800,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9807,7 +9808,7 @@
         <v>334</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9815,7 +9816,7 @@
         <v>335</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9823,7 +9824,7 @@
         <v>336</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9831,7 +9832,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9839,7 +9840,7 @@
         <v>337</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9847,7 +9848,7 @@
         <v>339</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9855,7 +9856,7 @@
         <v>340</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9863,7 +9864,7 @@
         <v>509</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9871,7 +9872,7 @@
         <v>89</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9879,7 +9880,7 @@
         <v>375</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9887,7 +9888,7 @@
         <v>376</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9895,7 +9896,7 @@
         <v>379</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9903,7 +9904,7 @@
         <v>90</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9911,7 +9912,7 @@
         <v>535</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9919,7 +9920,7 @@
         <v>536</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9927,7 +9928,7 @@
         <v>91</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9935,7 +9936,7 @@
         <v>380</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9943,7 +9944,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9951,7 +9952,7 @@
         <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -9975,7 +9976,7 @@
         <v>96</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9983,7 +9984,7 @@
         <v>540</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9991,7 +9992,7 @@
         <v>541</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9999,7 +10000,7 @@
         <v>542</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10007,7 +10008,7 @@
         <v>543</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10015,7 +10016,7 @@
         <v>547</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10031,7 +10032,7 @@
         <v>97</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10039,7 +10040,7 @@
         <v>98</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10047,7 +10048,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10055,7 +10056,7 @@
         <v>101</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10063,7 +10064,7 @@
         <v>100</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10071,7 +10072,7 @@
         <v>102</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10079,7 +10080,7 @@
         <v>103</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10087,7 +10088,7 @@
         <v>104</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10095,7 +10096,7 @@
         <v>105</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10103,7 +10104,7 @@
         <v>500</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10111,7 +10112,7 @@
         <v>501</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10119,7 +10120,7 @@
         <v>106</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10127,7 +10128,7 @@
         <v>107</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10135,7 +10136,7 @@
         <v>165</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -10143,7 +10144,7 @@
         <v>537</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10151,7 +10152,7 @@
         <v>108</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -10159,7 +10160,7 @@
         <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10167,7 +10168,7 @@
         <v>110</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10175,7 +10176,7 @@
         <v>166</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10183,7 +10184,7 @@
         <v>167</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10191,7 +10192,7 @@
         <v>168</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10199,7 +10200,7 @@
         <v>552</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10215,7 +10216,7 @@
         <v>111</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10223,7 +10224,7 @@
         <v>506</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -10231,7 +10232,7 @@
         <v>507</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -10247,7 +10248,7 @@
         <v>512</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10255,7 +10256,7 @@
         <v>112</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10263,7 +10264,7 @@
         <v>169</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10271,7 +10272,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10279,7 +10280,7 @@
         <v>171</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10287,7 +10288,7 @@
         <v>113</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10295,7 +10296,7 @@
         <v>114</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10303,7 +10304,7 @@
         <v>266</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10311,7 +10312,7 @@
         <v>559</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10319,7 +10320,7 @@
         <v>115</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10327,7 +10328,7 @@
         <v>518</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10335,7 +10336,7 @@
         <v>116</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10343,7 +10344,7 @@
         <v>516</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10351,7 +10352,7 @@
         <v>117</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10359,7 +10360,7 @@
         <v>519</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10367,7 +10368,7 @@
         <v>520</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10375,7 +10376,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10383,7 +10384,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -10391,7 +10392,7 @@
         <v>562</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10399,7 +10400,7 @@
         <v>563</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10407,7 +10408,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10415,7 +10416,7 @@
         <v>555</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10423,7 +10424,7 @@
         <v>554</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10431,7 +10432,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10439,7 +10440,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10447,7 +10448,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10455,7 +10456,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10463,7 +10464,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10471,7 +10472,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10479,7 +10480,7 @@
         <v>517</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10487,7 +10488,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10495,7 +10496,7 @@
         <v>560</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10503,7 +10504,7 @@
         <v>561</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10511,7 +10512,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10519,7 +10520,7 @@
         <v>604</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10527,7 +10528,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10535,7 +10536,7 @@
         <v>578</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10543,7 +10544,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10551,7 +10552,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10559,7 +10560,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10567,7 +10568,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10575,7 +10576,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10583,7 +10584,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -10591,7 +10592,7 @@
         <v>565</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10599,7 +10600,7 @@
         <v>566</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10607,7 +10608,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10615,7 +10616,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10623,7 +10624,7 @@
         <v>564</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10631,7 +10632,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10639,7 +10640,7 @@
         <v>579</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10647,7 +10648,7 @@
         <v>580</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10655,7 +10656,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10663,7 +10664,7 @@
         <v>581</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10671,7 +10672,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10679,7 +10680,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10687,7 +10688,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10695,7 +10696,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -10711,7 +10712,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10719,7 +10720,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10735,7 +10736,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10743,7 +10744,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10751,7 +10752,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10767,7 +10768,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10775,7 +10776,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10783,7 +10784,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10791,7 +10792,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10799,7 +10800,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10807,7 +10808,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10815,7 +10816,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10823,7 +10824,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10831,7 +10832,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10839,7 +10840,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10847,7 +10848,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10855,7 +10856,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10863,7 +10864,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10871,7 +10872,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10879,7 +10880,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10887,7 +10888,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10895,7 +10896,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10903,7 +10904,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10911,7 +10912,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10919,7 +10920,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10927,7 +10928,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10935,7 +10936,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10943,7 +10944,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10951,7 +10952,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10959,7 +10960,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10967,7 +10968,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10975,7 +10976,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10991,7 +10992,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10999,7 +11000,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11007,7 +11008,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11023,7 +11024,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11031,7 +11032,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11039,7 +11040,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11047,7 +11048,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11055,7 +11056,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11063,7 +11064,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11071,7 +11072,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11079,7 +11080,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11087,7 +11088,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11095,7 +11096,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11103,7 +11104,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -11111,7 +11112,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11127,7 +11128,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11135,7 +11136,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11143,7 +11144,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11151,7 +11152,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11159,7 +11160,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11167,7 +11168,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="370.9" x14ac:dyDescent="0.25">
@@ -11175,7 +11176,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11191,7 +11192,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11199,7 +11200,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="299.55" x14ac:dyDescent="0.25">
@@ -11207,7 +11208,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11215,7 +11216,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11223,7 +11224,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11231,7 +11232,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11239,7 +11240,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11247,7 +11248,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11255,7 +11256,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11263,7 +11264,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11271,7 +11272,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11279,7 +11280,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11287,7 +11288,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11303,7 +11304,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11311,7 +11312,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11319,7 +11320,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11335,7 +11336,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11343,7 +11344,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11351,7 +11352,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11367,7 +11368,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11375,7 +11376,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11383,7 +11384,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11391,7 +11392,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11399,7 +11400,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11407,7 +11408,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11415,7 +11416,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11423,7 +11424,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11431,7 +11432,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11447,7 +11448,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11455,7 +11456,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11463,7 +11464,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11471,7 +11472,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11479,7 +11480,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11487,7 +11488,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11495,7 +11496,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11503,7 +11504,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11511,7 +11512,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11519,7 +11520,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11527,7 +11528,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11535,7 +11536,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11543,7 +11544,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11551,7 +11552,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11559,7 +11560,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11567,7 +11568,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11575,7 +11576,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11583,7 +11584,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11591,7 +11592,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11599,7 +11600,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11607,7 +11608,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11615,7 +11616,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11663,7 +11664,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11671,7 +11672,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11679,7 +11680,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11687,7 +11688,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11695,7 +11696,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11703,7 +11704,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11711,7 +11712,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11719,7 +11720,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11791,7 +11792,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11799,7 +11800,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11807,7 +11808,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11815,7 +11816,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11823,7 +11824,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11831,7 +11832,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11839,7 +11840,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11847,7 +11848,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11855,7 +11856,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11863,7 +11864,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11871,7 +11872,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11879,7 +11880,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11887,7 +11888,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11895,7 +11896,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11903,7 +11904,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11911,7 +11912,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11919,7 +11920,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11927,7 +11928,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11935,7 +11936,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11943,7 +11944,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11951,7 +11952,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="285.3" x14ac:dyDescent="0.25">
@@ -11959,7 +11960,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11967,7 +11968,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11975,7 +11976,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11983,7 +11984,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11991,7 +11992,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11999,7 +12000,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12007,7 +12008,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12015,7 +12016,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12023,7 +12024,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12031,7 +12032,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12039,7 +12040,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12047,7 +12048,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12055,7 +12056,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12063,7 +12064,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12071,7 +12072,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12079,7 +12080,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12087,7 +12088,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12095,7 +12096,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12103,7 +12104,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12111,7 +12112,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -12119,7 +12120,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12127,7 +12128,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12135,7 +12136,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12143,7 +12144,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12151,7 +12152,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12159,7 +12160,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12167,7 +12168,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12175,7 +12176,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12183,7 +12184,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12191,7 +12192,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12207,7 +12208,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -12255,7 +12256,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12263,7 +12264,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12271,7 +12272,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12279,7 +12280,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12287,7 +12288,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12295,7 +12296,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12303,7 +12304,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12311,7 +12312,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12319,7 +12320,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12327,7 +12328,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12335,7 +12336,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12343,7 +12344,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12351,7 +12352,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12359,7 +12360,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12367,7 +12368,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12375,7 +12376,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12383,7 +12384,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12391,7 +12392,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12399,7 +12400,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12407,7 +12408,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12415,7 +12416,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12423,7 +12424,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12431,7 +12432,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12439,7 +12440,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -12447,7 +12448,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12455,7 +12456,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12463,7 +12464,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12471,7 +12472,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12479,7 +12480,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12487,7 +12488,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12495,7 +12496,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12503,7 +12504,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12511,7 +12512,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12519,7 +12520,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12527,7 +12528,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12535,7 +12536,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12543,7 +12544,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12551,7 +12552,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12559,7 +12560,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12567,7 +12568,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12575,7 +12576,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12583,7 +12584,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12591,7 +12592,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12599,7 +12600,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12607,7 +12608,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12615,7 +12616,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12623,7 +12624,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12631,7 +12632,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12639,7 +12640,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12663,7 +12664,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12671,7 +12672,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12679,7 +12680,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12687,7 +12688,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12695,7 +12696,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12703,7 +12704,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12711,7 +12712,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12719,7 +12720,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12727,7 +12728,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12735,7 +12736,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12743,7 +12744,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12775,7 +12776,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12823,7 +12824,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12831,7 +12832,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12847,7 +12848,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12855,7 +12856,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12863,7 +12864,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12871,7 +12872,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12919,7 +12920,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12927,7 +12928,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12935,7 +12936,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12943,7 +12944,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12951,7 +12952,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12959,7 +12960,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12967,7 +12968,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12975,7 +12976,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12983,7 +12984,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12991,7 +12992,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12999,7 +13000,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13007,7 +13008,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13015,7 +13016,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13031,7 +13032,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13039,7 +13040,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13047,7 +13048,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13055,7 +13056,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13063,7 +13064,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13071,7 +13072,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13079,7 +13080,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13095,7 +13096,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13103,7 +13104,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13111,7 +13112,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13119,7 +13120,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13135,7 +13136,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13143,7 +13144,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13151,7 +13152,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13159,7 +13160,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13167,7 +13168,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13175,7 +13176,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13199,7 +13200,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13207,7 +13208,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13215,7 +13216,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13239,7 +13240,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13247,7 +13248,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13255,7 +13256,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Changes: Updated description for e212n. Updated descriptin in the IconDisplayDialog.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFAB05BA-0F6A-4979-B1F9-71937C92DAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10429F6D-99BA-4342-AB82-D24B2815E07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -7299,15 +7299,6 @@
                    &lt;InlineUIContainer&gt;&lt;Image Source='../images/LightningScene.gif' Name='Temple' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e212n Staff of Command&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the
- &lt;InlineUIContainer&gt;&lt;Button Content='Tragoth River' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;In the meantime, you are given a pair of warrior monks who have combat skill 5 and endurance 6. The monks have mounts and join your parrty to help with your journey northward. Click image to continue.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                  &lt;InlineUIContainer&gt;&lt;Image Source='../images/Staff.gif' Name='EncounterEnd' Height='300' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e213 Rafting the Rivers&lt;/Bold&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r213' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You are using raft travel along the river. Your speed is  three hexsides per day downriver or two hexsides per day upriver. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, the raft halts for the night, and you camp on either hex adjacent to the hexside where travel ended. After traveling the hexsides, check once for a travel event
@@ -8135,6 +8126,15 @@
  6 - &lt;InlineUIContainer&gt;&lt;Button Content='e190' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;
         &lt;InlineUIContainer&gt;&lt;Image Name='E038EncounterRoll' Source='../images/Stone.gif' Height='280'  Width='525'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e212n Staff of Command&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the
+ &lt;InlineUIContainer&gt;&lt;Button Content='Tragoth River' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;In the meantime, you are given a pair of warrior monks who have combat skill 5 and endurance 6. The monks have mounts and join your party to help with your journey northward. Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                  &lt;InlineUIContainer&gt;&lt;Image Source='../images/Staff.gif' Name='EncounterEnd' Height='300' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8529,8 +8529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="B507" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B509" sqref="B509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8552,7 +8552,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8584,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8592,7 +8592,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9472,7 +9472,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9944,7 +9944,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10376,7 +10376,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10464,7 +10464,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10472,7 +10472,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10768,7 +10768,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11208,7 +11208,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11456,7 +11456,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11864,7 +11864,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12000,7 +12000,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12168,7 +12168,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12448,7 +12448,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12456,7 +12456,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12464,7 +12464,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12560,7 +12560,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12600,7 +12600,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1102</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12608,7 +12608,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12616,7 +12616,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12624,7 +12624,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12632,7 +12632,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12640,7 +12640,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12664,7 +12664,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12672,7 +12672,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12680,7 +12680,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12696,7 +12696,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12704,7 +12704,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12712,7 +12712,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12720,7 +12720,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12728,7 +12728,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12736,7 +12736,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12744,7 +12744,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12776,7 +12776,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12824,7 +12824,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12832,7 +12832,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12848,7 +12848,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12856,7 +12856,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12864,7 +12864,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12872,7 +12872,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12920,7 +12920,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12928,7 +12928,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12936,7 +12936,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12944,7 +12944,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12952,7 +12952,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12960,7 +12960,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12968,7 +12968,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12976,7 +12976,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12984,7 +12984,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12992,7 +12992,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13008,7 +13008,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13016,7 +13016,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13032,7 +13032,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13040,7 +13040,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13048,7 +13048,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13056,7 +13056,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13064,7 +13064,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13072,7 +13072,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13080,7 +13080,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13096,7 +13096,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13104,7 +13104,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13112,7 +13112,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13120,7 +13120,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13136,7 +13136,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13144,7 +13144,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13152,7 +13152,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13160,7 +13160,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13168,7 +13168,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13176,7 +13176,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13200,7 +13200,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13208,7 +13208,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13216,7 +13216,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13240,7 +13240,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13248,7 +13248,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13256,7 +13256,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
e023: fix description for die roll one. Turn on LE_COMBAT_WIZARD log level.
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10429F6D-99BA-4342-AB82-D24B2815E07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538A984-DB40-4065-89F5-5EC29EA8B9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -3482,19 +3482,6 @@
                                         &lt;InlineUIContainer&gt;&lt;Image Name='E023EncounterEvade'  Source='../images/Wizard.gif' Height='280'  Width='225' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e023c Fight Wizard&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die: 
-&lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e305' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Surprise&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e306' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Attacked &lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e024' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 and 4 - Wizard Attack&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e308' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Surprised&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='e307' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Attacked
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='E023EncounterFight'  Source='../images/Wizard.gif' Height='280'  Width='225' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;e024 Wizard Attack&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;A wizard attempts to use magic and take control of you and your party. Roll one die and  If the result equals or exceeds your wit and wiles, his attack is successful. If successful, see
  &lt;InlineUIContainer&gt;&lt;Button Content='e024a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -8135,6 +8122,19 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;In the meantime, you are given a pair of warrior monks who have combat skill 5 and endurance 6. The monks have mounts and join your party to help with your journey northward. Click image to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Staff.gif' Name='EncounterEnd' Height='300' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e023c Fight Wizard&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; Roll one die: 
+&lt;InlineUIContainer&gt;&lt;Image Source='../images/dieRoll.gif' Name='DieRoll' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e305' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 1 Attack&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e306' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 2 Attacked &lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e024' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 3 and 4 - Wizard Attack&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e308' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 5 Surprised&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='e307' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6 Attacked
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='E023EncounterFight'  Source='../images/Wizard.gif' Height='280'  Width='225' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -8529,8 +8529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B507" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B509" sqref="B509"/>
+    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8552,7 +8552,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -8584,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8592,7 +8592,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9248,7 +9248,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>737</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9256,7 +9256,7 @@
         <v>58</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9264,7 +9264,7 @@
         <v>523</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9272,7 +9272,7 @@
         <v>524</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9280,7 +9280,7 @@
         <v>527</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9288,7 +9288,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9296,7 +9296,7 @@
         <v>556</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9304,7 +9304,7 @@
         <v>60</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9312,7 +9312,7 @@
         <v>522</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9320,7 +9320,7 @@
         <v>61</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9328,7 +9328,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9336,7 +9336,7 @@
         <v>341</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9344,7 +9344,7 @@
         <v>63</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -9352,7 +9352,7 @@
         <v>64</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9360,7 +9360,7 @@
         <v>65</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -9368,7 +9368,7 @@
         <v>66</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9376,7 +9376,7 @@
         <v>329</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9384,7 +9384,7 @@
         <v>67</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9392,7 +9392,7 @@
         <v>386</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9400,7 +9400,7 @@
         <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9408,7 +9408,7 @@
         <v>342</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9416,7 +9416,7 @@
         <v>387</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9424,7 +9424,7 @@
         <v>69</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9432,7 +9432,7 @@
         <v>390</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9440,7 +9440,7 @@
         <v>391</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9448,7 +9448,7 @@
         <v>70</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -9456,7 +9456,7 @@
         <v>343</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9464,7 +9464,7 @@
         <v>259</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9472,7 +9472,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9480,7 +9480,7 @@
         <v>72</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9488,7 +9488,7 @@
         <v>73</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9504,7 +9504,7 @@
         <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9520,7 +9520,7 @@
         <v>324</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9528,7 +9528,7 @@
         <v>621</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -9536,7 +9536,7 @@
         <v>76</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9544,7 +9544,7 @@
         <v>77</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -9568,7 +9568,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9576,7 +9576,7 @@
         <v>349</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9584,7 +9584,7 @@
         <v>350</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9592,7 +9592,7 @@
         <v>79</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9600,7 +9600,7 @@
         <v>346</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9608,7 +9608,7 @@
         <v>347</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9616,7 +9616,7 @@
         <v>80</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9624,7 +9624,7 @@
         <v>81</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9632,7 +9632,7 @@
         <v>568</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9640,7 +9640,7 @@
         <v>569</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9648,7 +9648,7 @@
         <v>570</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9656,7 +9656,7 @@
         <v>571</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9664,7 +9664,7 @@
         <v>572</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9672,7 +9672,7 @@
         <v>573</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9680,7 +9680,7 @@
         <v>574</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9688,7 +9688,7 @@
         <v>575</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9696,7 +9696,7 @@
         <v>576</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9704,7 +9704,7 @@
         <v>577</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9712,7 +9712,7 @@
         <v>82</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9720,7 +9720,7 @@
         <v>83</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -9728,7 +9728,7 @@
         <v>601</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -9736,7 +9736,7 @@
         <v>84</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9744,7 +9744,7 @@
         <v>85</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9752,7 +9752,7 @@
         <v>425</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9760,7 +9760,7 @@
         <v>634</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9768,7 +9768,7 @@
         <v>86</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9776,7 +9776,7 @@
         <v>87</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9784,7 +9784,7 @@
         <v>333</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9792,7 +9792,7 @@
         <v>370</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="328.1" x14ac:dyDescent="0.25">
@@ -9800,7 +9800,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9808,7 +9808,7 @@
         <v>334</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9816,7 +9816,7 @@
         <v>335</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9824,7 +9824,7 @@
         <v>336</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9832,7 +9832,7 @@
         <v>338</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9840,7 +9840,7 @@
         <v>337</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9848,7 +9848,7 @@
         <v>339</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9856,7 +9856,7 @@
         <v>340</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -9864,7 +9864,7 @@
         <v>509</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9872,7 +9872,7 @@
         <v>89</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9880,7 +9880,7 @@
         <v>375</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9888,7 +9888,7 @@
         <v>376</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -9896,7 +9896,7 @@
         <v>379</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -9904,7 +9904,7 @@
         <v>90</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -9912,7 +9912,7 @@
         <v>535</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9920,7 +9920,7 @@
         <v>536</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -9928,7 +9928,7 @@
         <v>91</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -9936,7 +9936,7 @@
         <v>380</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9944,7 +9944,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -9952,7 +9952,7 @@
         <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -9976,7 +9976,7 @@
         <v>96</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -9984,7 +9984,7 @@
         <v>540</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -9992,7 +9992,7 @@
         <v>541</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10000,7 +10000,7 @@
         <v>542</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10008,7 +10008,7 @@
         <v>543</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10016,7 +10016,7 @@
         <v>547</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10032,7 +10032,7 @@
         <v>97</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10040,7 +10040,7 @@
         <v>98</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10048,7 +10048,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10056,7 +10056,7 @@
         <v>101</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10064,7 +10064,7 @@
         <v>100</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10072,7 +10072,7 @@
         <v>102</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10080,7 +10080,7 @@
         <v>103</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10088,7 +10088,7 @@
         <v>104</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10096,7 +10096,7 @@
         <v>105</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10104,7 +10104,7 @@
         <v>500</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10112,7 +10112,7 @@
         <v>501</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10120,7 +10120,7 @@
         <v>106</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10128,7 +10128,7 @@
         <v>107</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10136,7 +10136,7 @@
         <v>165</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -10144,7 +10144,7 @@
         <v>537</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10152,7 +10152,7 @@
         <v>108</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -10160,7 +10160,7 @@
         <v>109</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10168,7 +10168,7 @@
         <v>110</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10176,7 +10176,7 @@
         <v>166</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10184,7 +10184,7 @@
         <v>167</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10192,7 +10192,7 @@
         <v>168</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10200,7 +10200,7 @@
         <v>552</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10216,7 +10216,7 @@
         <v>111</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10224,7 +10224,7 @@
         <v>506</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -10232,7 +10232,7 @@
         <v>507</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -10248,7 +10248,7 @@
         <v>512</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10256,7 +10256,7 @@
         <v>112</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10264,7 +10264,7 @@
         <v>169</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10272,7 +10272,7 @@
         <v>170</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10280,7 +10280,7 @@
         <v>171</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10288,7 +10288,7 @@
         <v>113</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10296,7 +10296,7 @@
         <v>114</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10304,7 +10304,7 @@
         <v>266</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10312,7 +10312,7 @@
         <v>559</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10320,7 +10320,7 @@
         <v>115</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10328,7 +10328,7 @@
         <v>518</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10336,7 +10336,7 @@
         <v>116</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10344,7 +10344,7 @@
         <v>516</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10352,7 +10352,7 @@
         <v>117</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10360,7 +10360,7 @@
         <v>519</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10368,7 +10368,7 @@
         <v>520</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10376,7 +10376,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10384,7 +10384,7 @@
         <v>118</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -10392,7 +10392,7 @@
         <v>562</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10400,7 +10400,7 @@
         <v>563</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10408,7 +10408,7 @@
         <v>119</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10416,7 +10416,7 @@
         <v>555</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10424,7 +10424,7 @@
         <v>554</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10432,7 +10432,7 @@
         <v>120</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10440,7 +10440,7 @@
         <v>172</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10448,7 +10448,7 @@
         <v>173</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10456,7 +10456,7 @@
         <v>174</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10464,7 +10464,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10472,7 +10472,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10480,7 +10480,7 @@
         <v>517</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10488,7 +10488,7 @@
         <v>123</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10496,7 +10496,7 @@
         <v>560</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10504,7 +10504,7 @@
         <v>561</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10512,7 +10512,7 @@
         <v>124</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10520,7 +10520,7 @@
         <v>604</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10528,7 +10528,7 @@
         <v>125</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10536,7 +10536,7 @@
         <v>578</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10544,7 +10544,7 @@
         <v>126</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10552,7 +10552,7 @@
         <v>127</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10560,7 +10560,7 @@
         <v>128</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10568,7 +10568,7 @@
         <v>129</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10576,7 +10576,7 @@
         <v>130</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10584,7 +10584,7 @@
         <v>131</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -10592,7 +10592,7 @@
         <v>565</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10600,7 +10600,7 @@
         <v>566</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10608,7 +10608,7 @@
         <v>132</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10616,7 +10616,7 @@
         <v>133</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10624,7 +10624,7 @@
         <v>564</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -10632,7 +10632,7 @@
         <v>134</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10640,7 +10640,7 @@
         <v>579</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10648,7 +10648,7 @@
         <v>580</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10656,7 +10656,7 @@
         <v>135</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -10664,7 +10664,7 @@
         <v>581</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10672,7 +10672,7 @@
         <v>136</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10680,7 +10680,7 @@
         <v>137</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10688,7 +10688,7 @@
         <v>232</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10696,7 +10696,7 @@
         <v>233</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -10712,7 +10712,7 @@
         <v>234</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10720,7 +10720,7 @@
         <v>235</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10736,7 +10736,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10744,7 +10744,7 @@
         <v>240</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10752,7 +10752,7 @@
         <v>241</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10768,7 +10768,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -10776,7 +10776,7 @@
         <v>237</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10784,7 +10784,7 @@
         <v>238</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10792,7 +10792,7 @@
         <v>141</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10800,7 +10800,7 @@
         <v>142</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10808,7 +10808,7 @@
         <v>143</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -10816,7 +10816,7 @@
         <v>144</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10824,7 +10824,7 @@
         <v>242</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10832,7 +10832,7 @@
         <v>145</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10840,7 +10840,7 @@
         <v>146</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10848,7 +10848,7 @@
         <v>147</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10856,7 +10856,7 @@
         <v>148</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -10864,7 +10864,7 @@
         <v>149</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10872,7 +10872,7 @@
         <v>592</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10880,7 +10880,7 @@
         <v>591</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -10888,7 +10888,7 @@
         <v>593</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10896,7 +10896,7 @@
         <v>150</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10904,7 +10904,7 @@
         <v>594</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -10912,7 +10912,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10920,7 +10920,7 @@
         <v>243</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10928,7 +10928,7 @@
         <v>244</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10936,7 +10936,7 @@
         <v>245</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10944,7 +10944,7 @@
         <v>152</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10952,7 +10952,7 @@
         <v>153</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -10960,7 +10960,7 @@
         <v>154</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -10968,7 +10968,7 @@
         <v>155</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -10976,7 +10976,7 @@
         <v>156</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -10992,7 +10992,7 @@
         <v>246</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11000,7 +11000,7 @@
         <v>247</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11008,7 +11008,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11024,7 +11024,7 @@
         <v>159</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11032,7 +11032,7 @@
         <v>160</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11040,7 +11040,7 @@
         <v>161</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11048,7 +11048,7 @@
         <v>162</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11056,7 +11056,7 @@
         <v>587</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11064,7 +11064,7 @@
         <v>588</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11072,7 +11072,7 @@
         <v>589</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11080,7 +11080,7 @@
         <v>163</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11088,7 +11088,7 @@
         <v>164</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11096,7 +11096,7 @@
         <v>175</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11104,7 +11104,7 @@
         <v>176</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -11112,7 +11112,7 @@
         <v>177</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11128,7 +11128,7 @@
         <v>411</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11136,7 +11136,7 @@
         <v>412</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11144,7 +11144,7 @@
         <v>413</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11152,7 +11152,7 @@
         <v>414</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11160,7 +11160,7 @@
         <v>415</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11168,7 +11168,7 @@
         <v>600</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="370.9" x14ac:dyDescent="0.25">
@@ -11176,7 +11176,7 @@
         <v>178</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11192,7 +11192,7 @@
         <v>423</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11200,7 +11200,7 @@
         <v>424</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="299.55" x14ac:dyDescent="0.25">
@@ -11208,7 +11208,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11216,7 +11216,7 @@
         <v>249</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11224,7 +11224,7 @@
         <v>250</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11232,7 +11232,7 @@
         <v>251</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11240,7 +11240,7 @@
         <v>252</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11248,7 +11248,7 @@
         <v>253</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11256,7 +11256,7 @@
         <v>538</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11264,7 +11264,7 @@
         <v>539</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11272,7 +11272,7 @@
         <v>180</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11280,7 +11280,7 @@
         <v>181</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11288,7 +11288,7 @@
         <v>384</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11304,7 +11304,7 @@
         <v>609</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11312,7 +11312,7 @@
         <v>183</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11320,7 +11320,7 @@
         <v>184</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -11336,7 +11336,7 @@
         <v>185</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11344,7 +11344,7 @@
         <v>186</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11352,7 +11352,7 @@
         <v>187</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11368,7 +11368,7 @@
         <v>188</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11376,7 +11376,7 @@
         <v>189</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11384,7 +11384,7 @@
         <v>381</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11392,7 +11392,7 @@
         <v>382</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11400,7 +11400,7 @@
         <v>190</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11408,7 +11408,7 @@
         <v>191</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11416,7 +11416,7 @@
         <v>192</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11424,7 +11424,7 @@
         <v>461</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11432,7 +11432,7 @@
         <v>193</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11448,7 +11448,7 @@
         <v>332</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11456,7 +11456,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -11464,7 +11464,7 @@
         <v>612</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11472,7 +11472,7 @@
         <v>614</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11480,7 +11480,7 @@
         <v>615</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11488,7 +11488,7 @@
         <v>616</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11496,7 +11496,7 @@
         <v>617</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11504,7 +11504,7 @@
         <v>618</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11512,7 +11512,7 @@
         <v>619</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11520,7 +11520,7 @@
         <v>194</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -11528,7 +11528,7 @@
         <v>195</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11536,7 +11536,7 @@
         <v>607</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11544,7 +11544,7 @@
         <v>196</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -11552,7 +11552,7 @@
         <v>327</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11560,7 +11560,7 @@
         <v>197</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11568,7 +11568,7 @@
         <v>483</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11576,7 +11576,7 @@
         <v>198</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11584,7 +11584,7 @@
         <v>199</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11592,7 +11592,7 @@
         <v>200</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11600,7 +11600,7 @@
         <v>201</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11608,7 +11608,7 @@
         <v>202</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11616,7 +11616,7 @@
         <v>203</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11664,7 +11664,7 @@
         <v>204</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11672,7 +11672,7 @@
         <v>455</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11680,7 +11680,7 @@
         <v>456</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11688,7 +11688,7 @@
         <v>457</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11696,7 +11696,7 @@
         <v>458</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -11704,7 +11704,7 @@
         <v>459</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11712,7 +11712,7 @@
         <v>460</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11720,7 +11720,7 @@
         <v>205</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -11792,7 +11792,7 @@
         <v>207</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -11800,7 +11800,7 @@
         <v>208</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11808,7 +11808,7 @@
         <v>209</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11816,7 +11816,7 @@
         <v>472</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11824,7 +11824,7 @@
         <v>473</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11832,7 +11832,7 @@
         <v>474</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11840,7 +11840,7 @@
         <v>475</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11848,7 +11848,7 @@
         <v>476</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11856,7 +11856,7 @@
         <v>477</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -11864,7 +11864,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -11872,7 +11872,7 @@
         <v>210</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11880,7 +11880,7 @@
         <v>465</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11888,7 +11888,7 @@
         <v>466</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11896,7 +11896,7 @@
         <v>467</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11904,7 +11904,7 @@
         <v>468</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11912,7 +11912,7 @@
         <v>469</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11920,7 +11920,7 @@
         <v>470</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11928,7 +11928,7 @@
         <v>471</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -11936,7 +11936,7 @@
         <v>606</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -11944,7 +11944,7 @@
         <v>211</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -11952,7 +11952,7 @@
         <v>212</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="285.3" x14ac:dyDescent="0.25">
@@ -11960,7 +11960,7 @@
         <v>416</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11968,7 +11968,7 @@
         <v>417</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11976,7 +11976,7 @@
         <v>418</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -11984,7 +11984,7 @@
         <v>419</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -11992,7 +11992,7 @@
         <v>213</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12000,7 +12000,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12008,7 +12008,7 @@
         <v>215</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12016,7 +12016,7 @@
         <v>216</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12024,7 +12024,7 @@
         <v>217</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12032,7 +12032,7 @@
         <v>218</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12040,7 +12040,7 @@
         <v>219</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12048,7 +12048,7 @@
         <v>220</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12056,7 +12056,7 @@
         <v>221</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12064,7 +12064,7 @@
         <v>222</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12072,7 +12072,7 @@
         <v>223</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12080,7 +12080,7 @@
         <v>224</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12088,7 +12088,7 @@
         <v>328</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12096,7 +12096,7 @@
         <v>383</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12104,7 +12104,7 @@
         <v>225</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12112,7 +12112,7 @@
         <v>226</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -12120,7 +12120,7 @@
         <v>227</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12128,7 +12128,7 @@
         <v>228</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12136,7 +12136,7 @@
         <v>605</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12144,7 +12144,7 @@
         <v>229</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12152,7 +12152,7 @@
         <v>230</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12160,7 +12160,7 @@
         <v>231</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12168,7 +12168,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12176,7 +12176,7 @@
         <v>377</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12184,7 +12184,7 @@
         <v>378</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12192,7 +12192,7 @@
         <v>440</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12208,7 +12208,7 @@
         <v>525</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -12256,7 +12256,7 @@
         <v>590</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12264,7 +12264,7 @@
         <v>321</v>
       </c>
       <c r="B466" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12272,7 +12272,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="3" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12280,7 +12280,7 @@
         <v>392</v>
       </c>
       <c r="B468" s="3" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12288,7 +12288,7 @@
         <v>394</v>
       </c>
       <c r="B469" s="3" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12296,7 +12296,7 @@
         <v>395</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12304,7 +12304,7 @@
         <v>396</v>
       </c>
       <c r="B471" s="3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12312,7 +12312,7 @@
         <v>397</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12320,7 +12320,7 @@
         <v>398</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12328,7 +12328,7 @@
         <v>427</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12336,7 +12336,7 @@
         <v>428</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12344,7 +12344,7 @@
         <v>633</v>
       </c>
       <c r="B476" s="3" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12352,7 +12352,7 @@
         <v>429</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12360,7 +12360,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12368,7 +12368,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12376,7 +12376,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12384,7 +12384,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12392,7 +12392,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12400,7 +12400,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12408,7 +12408,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12416,7 +12416,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -12424,7 +12424,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -12432,7 +12432,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12440,7 +12440,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="256.75" x14ac:dyDescent="0.25">
@@ -12448,7 +12448,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12456,7 +12456,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12464,7 +12464,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -12472,7 +12472,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12480,7 +12480,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12488,7 +12488,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12496,7 +12496,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12504,7 +12504,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12512,7 +12512,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12520,7 +12520,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12528,7 +12528,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12536,7 +12536,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12544,7 +12544,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12552,7 +12552,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -12560,7 +12560,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12568,7 +12568,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12576,7 +12576,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -12584,7 +12584,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12592,7 +12592,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12600,7 +12600,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
@@ -12608,7 +12608,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12616,7 +12616,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12624,7 +12624,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12632,7 +12632,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12640,7 +12640,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12664,7 +12664,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12672,7 +12672,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12680,7 +12680,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12696,7 +12696,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12704,7 +12704,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12712,7 +12712,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12720,7 +12720,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12728,7 +12728,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12736,7 +12736,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -12744,7 +12744,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12776,7 +12776,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12824,7 +12824,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12832,7 +12832,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -12848,7 +12848,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12856,7 +12856,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12864,7 +12864,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12872,7 +12872,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12920,7 +12920,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12928,7 +12928,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12936,7 +12936,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12944,7 +12944,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
@@ -12952,7 +12952,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12960,7 +12960,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -12968,7 +12968,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -12976,7 +12976,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -12984,7 +12984,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -12992,7 +12992,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -13008,7 +13008,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13016,7 +13016,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13032,7 +13032,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13040,7 +13040,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13048,7 +13048,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13056,7 +13056,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
@@ -13064,7 +13064,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13072,7 +13072,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13080,7 +13080,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13096,7 +13096,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13104,7 +13104,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -13112,7 +13112,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13120,7 +13120,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13136,7 +13136,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13144,7 +13144,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
@@ -13152,7 +13152,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
@@ -13160,7 +13160,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="385.15" x14ac:dyDescent="0.25">
@@ -13168,7 +13168,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
@@ -13176,7 +13176,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13200,7 +13200,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13208,7 +13208,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -13216,7 +13216,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
@@ -13240,7 +13240,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
@@ -13248,7 +13248,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -13256,7 +13256,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change event 201a to fix label issue
</commit_message>
<xml_diff>
--- a/DesignDocs/Events.xlsx
+++ b/DesignDocs/Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6594FD7-5671-44A8-853E-8AC7C5A71091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B753465-AF56-4922-841A-ECC1E93D026E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -7012,14 +7012,6 @@
 12: &lt;InlineUIContainer&gt;&lt;Button Content='e210i' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - Porters and a local guide are available</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;e210a Freeman Available&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;A freeman joins your party at no cost (except food and lodging). He has a combat skill 3 and endurance 4. Choose image to click.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to not allow him to join:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='EncounterEnd' Source='../images/FoodDeny.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to not allow him to join:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='HireFreeman' Source='../images/Food.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;e210b Lancer Available&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;A lancer with a horse can be hired for 3 gold per day. He  has a combat skill of 5 and endurance of 5. Click one of images to continue.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to allow him to join:
@@ -8135,6 +8127,14 @@
 &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='Fight' Name='e112c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;   -&gt;  
 &lt;InlineUIContainer&gt;&lt;Button FontFamily='Courier New'  FontSize='12' Content='e112c'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;*If you select fly, see &lt;InlineUIContainer&gt;&lt;Button Content='r219' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for procedures for a follow move today and then consult the event listed. If you elect to follow, you must abandon all members of your party without winged mounts or ability to fly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;e210a Freeman Available&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A freeman joins your party at no cost (except food and lodging). He has a combat skill 3 and endurance 4. Choose image to click.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to not allow him to join:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='EncounterEnd' Source='../images/FoodDeny.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click to allow him to join:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;InlineUIContainer&gt;&lt;Image Name='HireFreeman' Source='../images/Food.gif' Height='100'  Width='100'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -8529,8 +8529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B295" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B297" sqref="B297"/>
+    <sheetView tabSelected="1" topLeftCell="B477" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B479" sqref="B479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8552,7 +8552,7 @@
         <v>254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="142.69999999999999" x14ac:dyDescent="0.25">
@@ -8584,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
@@ -8592,7 +8592,7 @@
         <v>653</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -9248,7 +9248,7 @@
         <v>57</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -9472,7 +9472,7 @@
         <v>71</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -9944,7 +9944,7 @@
         <v>92</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -10376,7 +10376,7 @@
         <v>521</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -10464,7 +10464,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -10472,7 +10472,7 @@
         <v>122</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -10768,7 +10768,7 @@
         <v>236</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -10912,7 +10912,7 @@
         <v>151</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -11208,7 +11208,7 @@
         <v>179</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -11456,7 +11456,7 @@
         <v>611</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -11864,7 +11864,7 @@
         <v>608</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12000,7 +12000,7 @@
         <v>214</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12168,7 +12168,7 @@
         <v>257</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12360,7 +12360,7 @@
         <v>430</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1074</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12368,7 +12368,7 @@
         <v>431</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12376,7 +12376,7 @@
         <v>432</v>
       </c>
       <c r="B480" s="3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12384,7 +12384,7 @@
         <v>433</v>
       </c>
       <c r="B481" s="3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12392,7 +12392,7 @@
         <v>434</v>
       </c>
       <c r="B482" s="3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12400,7 +12400,7 @@
         <v>435</v>
       </c>
       <c r="B483" s="3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12408,7 +12408,7 @@
         <v>436</v>
       </c>
       <c r="B484" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12416,7 +12416,7 @@
         <v>437</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -12424,7 +12424,7 @@
         <v>438</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -12432,7 +12432,7 @@
         <v>439</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12440,7 +12440,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="270" x14ac:dyDescent="0.25">
@@ -12448,7 +12448,7 @@
         <v>462</v>
       </c>
       <c r="B489" s="3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12456,7 +12456,7 @@
         <v>463</v>
       </c>
       <c r="B490" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12464,7 +12464,7 @@
         <v>464</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -12472,7 +12472,7 @@
         <v>544</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12480,7 +12480,7 @@
         <v>620</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12488,7 +12488,7 @@
         <v>484</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12496,7 +12496,7 @@
         <v>485</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12504,7 +12504,7 @@
         <v>486</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12512,7 +12512,7 @@
         <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12520,7 +12520,7 @@
         <v>488</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12528,7 +12528,7 @@
         <v>489</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12536,7 +12536,7 @@
         <v>490</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12544,7 +12544,7 @@
         <v>491</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12552,7 +12552,7 @@
         <v>492</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -12560,7 +12560,7 @@
         <v>493</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12568,7 +12568,7 @@
         <v>494</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12576,7 +12576,7 @@
         <v>495</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="506" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -12584,7 +12584,7 @@
         <v>496</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="507" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12592,7 +12592,7 @@
         <v>497</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="508" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12600,7 +12600,7 @@
         <v>498</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="509" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -12608,7 +12608,7 @@
         <v>585</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="510" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12616,7 +12616,7 @@
         <v>586</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="511" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12624,7 +12624,7 @@
         <v>499</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12632,7 +12632,7 @@
         <v>511</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12640,7 +12640,7 @@
         <v>420</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12664,7 +12664,7 @@
         <v>267</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="517" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12672,7 +12672,7 @@
         <v>268</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12680,7 +12680,7 @@
         <v>269</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>270</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12696,7 +12696,7 @@
         <v>271</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="521" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12704,7 +12704,7 @@
         <v>272</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="522" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12712,7 +12712,7 @@
         <v>273</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12720,7 +12720,7 @@
         <v>274</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12728,7 +12728,7 @@
         <v>275</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12736,7 +12736,7 @@
         <v>276</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -12744,7 +12744,7 @@
         <v>277</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12776,7 +12776,7 @@
         <v>315</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12824,7 +12824,7 @@
         <v>280</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12832,7 +12832,7 @@
         <v>281</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12848,7 +12848,7 @@
         <v>283</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12856,7 +12856,7 @@
         <v>284</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12864,7 +12864,7 @@
         <v>285</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12872,7 +12872,7 @@
         <v>286</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="543" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12920,7 +12920,7 @@
         <v>292</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="549" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12928,7 +12928,7 @@
         <v>293</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="550" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12936,7 +12936,7 @@
         <v>294</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="551" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12944,7 +12944,7 @@
         <v>295</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="552" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -12952,7 +12952,7 @@
         <v>296</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="553" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12960,7 +12960,7 @@
         <v>297</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -12968,7 +12968,7 @@
         <v>352</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -12976,7 +12976,7 @@
         <v>364</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="556" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -12984,7 +12984,7 @@
         <v>365</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="557" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -12992,7 +12992,7 @@
         <v>298</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="558" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>363</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="559" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -13008,7 +13008,7 @@
         <v>299</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="560" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13016,7 +13016,7 @@
         <v>353</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13032,7 +13032,7 @@
         <v>300</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13040,7 +13040,7 @@
         <v>301</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="564" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13048,7 +13048,7 @@
         <v>302</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="565" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13056,7 +13056,7 @@
         <v>303</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="566" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -13064,7 +13064,7 @@
         <v>362</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="567" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13072,7 +13072,7 @@
         <v>304</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="568" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13080,7 +13080,7 @@
         <v>360</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="569" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13096,7 +13096,7 @@
         <v>513</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="571" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13104,7 +13104,7 @@
         <v>305</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="572" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -13112,7 +13112,7 @@
         <v>357</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="573" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13120,7 +13120,7 @@
         <v>358</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13136,7 +13136,7 @@
         <v>514</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="576" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13144,7 +13144,7 @@
         <v>306</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="577" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -13152,7 +13152,7 @@
         <v>351</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="578" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -13160,7 +13160,7 @@
         <v>354</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="579" spans="1:2" ht="405" x14ac:dyDescent="0.25">
@@ -13168,7 +13168,7 @@
         <v>307</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="580" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -13176,7 +13176,7 @@
         <v>311</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="581" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13200,7 +13200,7 @@
         <v>348</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="584" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13208,7 +13208,7 @@
         <v>515</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -13216,7 +13216,7 @@
         <v>325</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="586" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -13240,7 +13240,7 @@
         <v>650</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="589" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -13248,7 +13248,7 @@
         <v>652</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="590" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -13256,7 +13256,7 @@
         <v>651</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>